<commit_message>
fix gantt order, update budget pie, update feedback tracking data and script
</commit_message>
<xml_diff>
--- a/xlsx/OTP_feedback_tracking_cleaned_no_pi.xlsx
+++ b/xlsx/OTP_feedback_tracking_cleaned_no_pi.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="423">
   <si>
     <t>Date Received</t>
   </si>
@@ -283,7 +283,7 @@
     <t>"It was very helpful and planned my trip well giving an idea what time I need to be there. THANK YOU!!"</t>
   </si>
   <si>
-    <t>Undesirable trip plan; Text planner form not functioning as expected</t>
+    <t>Undesirable trip plan; Text planner not functioning as expected</t>
   </si>
   <si>
     <t>"a first time visitor i found this planner to be astoundingly helpful"</t>
@@ -349,9 +349,6 @@
     <t>"Having a map showing the directions would also be great, seems like the natural next step."</t>
   </si>
   <si>
-    <t>Undesirable trip plan; Text planner not functioning as expected</t>
-  </si>
-  <si>
     <t>"Thank you for such a user friendly web site."</t>
   </si>
   <si>
@@ -364,6 +361,18 @@
     <t>"The trip planner website is fantastic! Very intuitive, uncluttered, and logically layed out. Bravo. Seriously."</t>
   </si>
   <si>
+    <t>Customer prefers a different transfer point</t>
+  </si>
+  <si>
+    <t>Trip plan is "To" Current Location</t>
+  </si>
+  <si>
+    <t>"travel screen much easier to use than last time"</t>
+  </si>
+  <si>
+    <t>Would like compass on maps</t>
+  </si>
+  <si>
     <t>Location outside district</t>
   </si>
   <si>
@@ -550,16 +559,13 @@
     <t>Unclear - maybe Incorrect address</t>
   </si>
   <si>
-    <t>No service to destination at required time of day</t>
-  </si>
-  <si>
-    <t>scheduling issue - the customer must've inadvertently planned a trip on the short line</t>
-  </si>
-  <si>
-    <t>scheduling issue - destination is on a morning/evening only route</t>
-  </si>
-  <si>
-    <t>Scheduling issue - trip planned before service begins on desired route</t>
+    <t>Scheduling issue; Destination is on a morning/evening only route</t>
+  </si>
+  <si>
+    <t>Scheduling issue; The customer inadvertently planned a trip on the short line</t>
+  </si>
+  <si>
+    <t>Scheduling issue; Trip planned before service begins on desired route</t>
   </si>
   <si>
     <t>Streetcar is not included; Drop downs not workings; Problems showing multiple closures for one stop</t>
@@ -586,6 +592,9 @@
     <t>Replicated bug - can't handle more than 1 interline</t>
   </si>
   <si>
+    <t>Scheduling issue; No weekend service on desired route</t>
+  </si>
+  <si>
     <t>Vancouver</t>
   </si>
   <si>
@@ -616,6 +625,9 @@
     <t>http://trimet.org/ride/planner_geocode.html?geo_type=from&amp;from=575%20NW%20Michelbook%20Ln%2C%20McMinnville%2C%20OR%2097128</t>
   </si>
   <si>
+    <t>http://ride.trimet.org/#/.</t>
+  </si>
+  <si>
     <t>http://trimet.org/ride/stop_select_geocode.html?place=Northeast%20130th%20Avenue%20Portland%2C%20OR%2097230</t>
   </si>
   <si>
@@ -814,6 +826,9 @@
     <t>http://trimet.org/#planner/results/from=8039+NE+FAILING+ST%2C+Portland%3A%3A45.551197%2C-122.58013&amp;to=NW+22nd+Ave+%26+W+Burnside+St%2C+Portland%3A%3A45.52332%2C-122.69636&amp;m=am&amp;walk=1260&amp;arr=A</t>
   </si>
   <si>
+    <t>http://trimet.org/schedules/w/t1096_0.htm.</t>
+  </si>
+  <si>
     <t>http://trimet.org/#/planner/results/itin_num=1&amp;from=Amtrak%20Union%20Station,%20Portland::45.529,-122.67669&amp;to=11321%20SW%20BASSWOOD%20CT,%20Tigard::45.44419,-122.79137&amp;Walk=1260&amp;Arr=D</t>
   </si>
   <si>
@@ -871,6 +886,9 @@
     <t>http://trimet.org/#planner/results/from=PCC+Rock+Creek+Main+Stop+S+(Stop+ID+4429)%3A%3A45.566013%2C-122.85943&amp;to=Willow+Creek+Transit+Center+E%2C+Hillsboro+(Stop+ID+9610)%3A%3A45.517307%2C-122.87002&amp;mode=TRAINISH%2CWALK&amp;m=pm&amp;walk=420&amp;arr=A</t>
   </si>
   <si>
+    <t>http://ride.trimet.org</t>
+  </si>
+  <si>
     <t>http://trimet.org/#/planner/results/itin_num=3&amp;from=2607%20SE%2035TH%20AVE,%20Portland::45.503998,-122.62888&amp;to=SW%20Broadway%20%26%20SW%20Mill%20St,%20Portland::45.512684,-122.68322&amp;Walk=420&amp;Arr=A</t>
   </si>
   <si>
@@ -1234,10 +1252,34 @@
     <t>http://trimet.org/#/planner/results/itin_num=1&amp;from=2090</t>
   </si>
   <si>
+    <t>http://trimet.org/#planner/results/from=SW+BEAVERTON+HILLSDALE+HWY+%26+SW+LAURELWOOD+AVE%3A%3A45.48623%2C-122.760879&amp;to=3326+SW+MARQUAM+HILL+RD%3A%3A45.499043%2C-122.694014&amp;walk=1260&amp;arr=D</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#planner/results/from=Tigard+Transit+Center%2C+Tigard%3A%3A45.430267%2C-122.76936&amp;to=4970+SW+GRIFFITH+DR%3A%3A45.483687%2C-122.7949&amp;m=pm&amp;walk=420&amp;arr=A</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#planner/results/from=1030+NE+102ND+AVE%2C+Portland%3A%3A45.530365%2C-122.55744&amp;to=7037+NE+Sandy+Blvd&amp;m=am&amp;walk=1260&amp;arr=A</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#planner/results/from=1511+SW+PARK+AVE%2C+PORTLAND%3A%3A45.514206%2C-122.68472&amp;to=1423+SE+HAWTHORNE+BLVD%2C+PORTLAND%3A%3A45.512432%2C-122.65196&amp;m=am&amp;walk=420&amp;arr=D</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=NW+5th+Ave+%26+NW+Everett+St%2C+Portland%3A%3A45.525223%2C-122.67548&amp;to=Current+Location%3A%3A45.52487187192392%2C-122.67620650266917&amp;m=am&amp;walk=1260&amp;arr=D</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#planner/results/from=2545+SW+TERWILLIGER+BLVD%2C+Portland%3A%3A45.50432%2C-122.68524&amp;to=11782+SW+BARNES+RD%2C+Portland%3A%3A45.51669%2C-122.79859&amp;m=pm&amp;walk=1260&amp;arr=A</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=1429+N+WEBSTER+ST%2C+Portland%3A%3A45.55985%2C-122.68187&amp;to=Clackamas+Town+Center+TC+%26+Clackamas+Town+Ctr%2C+Clackamas+County%3A%3A45.43555%2C-122.56904&amp;m=pm&amp;walk=1260&amp;arr=A</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#/planner/results/itin_num=1&amp;from=Amtrak</t>
+  </si>
+  <si>
+    <t>Weekday</t>
+  </si>
+  <si>
     <t>Saturday</t>
-  </si>
-  <si>
-    <t>Weekday</t>
   </si>
   <si>
     <t>Holiday</t>
@@ -1602,7 +1644,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I298"/>
+  <dimension ref="A1:I306"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1698,13 +1740,13 @@
         <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G4" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="H4" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1724,13 +1766,13 @@
         <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G5" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H5" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1749,6 +1791,12 @@
       <c r="E6" t="s">
         <v>25</v>
       </c>
+      <c r="H6" t="s">
+        <v>203</v>
+      </c>
+      <c r="I6" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1">
@@ -1807,7 +1855,7 @@
         <v>21</v>
       </c>
       <c r="H9" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1827,13 +1875,13 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G10" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="H10" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1870,13 +1918,13 @@
         <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G12" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="H12" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1896,7 +1944,7 @@
         <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1916,7 +1964,7 @@
         <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1956,13 +2004,13 @@
         <v>24</v>
       </c>
       <c r="F16" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G16" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="H16" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1999,7 +2047,7 @@
         <v>23</v>
       </c>
       <c r="F18" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2019,10 +2067,10 @@
         <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H19" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2042,13 +2090,13 @@
         <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G20" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="H20" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2068,10 +2116,10 @@
         <v>27</v>
       </c>
       <c r="F21" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H21" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2091,13 +2139,13 @@
         <v>24</v>
       </c>
       <c r="F22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G22" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="H22" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2117,13 +2165,13 @@
         <v>24</v>
       </c>
       <c r="F23" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G23" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="H23" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2143,7 +2191,7 @@
         <v>23</v>
       </c>
       <c r="F24" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2180,7 +2228,7 @@
         <v>34</v>
       </c>
       <c r="F26" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2200,10 +2248,10 @@
         <v>27</v>
       </c>
       <c r="F27" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="H27" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2223,10 +2271,10 @@
         <v>27</v>
       </c>
       <c r="F28" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H28" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2246,13 +2294,13 @@
         <v>24</v>
       </c>
       <c r="F29" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G29" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="H29" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2272,13 +2320,13 @@
         <v>24</v>
       </c>
       <c r="F30" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G30" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="H30" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2315,13 +2363,13 @@
         <v>24</v>
       </c>
       <c r="F32" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G32" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="H32" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2341,10 +2389,10 @@
         <v>27</v>
       </c>
       <c r="F33" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H33" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2381,10 +2429,10 @@
         <v>24</v>
       </c>
       <c r="F35" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G35" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2404,10 +2452,10 @@
         <v>24</v>
       </c>
       <c r="F36" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G36" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2427,10 +2475,10 @@
         <v>27</v>
       </c>
       <c r="F37" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H37" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2484,10 +2532,10 @@
         <v>27</v>
       </c>
       <c r="F40" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H40" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2507,13 +2555,13 @@
         <v>24</v>
       </c>
       <c r="F41" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G41" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="H41" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2533,13 +2581,13 @@
         <v>24</v>
       </c>
       <c r="F42" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G42" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="H42" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2559,7 +2607,7 @@
         <v>38</v>
       </c>
       <c r="F43" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2579,10 +2627,10 @@
         <v>27</v>
       </c>
       <c r="F44" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H44" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2602,10 +2650,10 @@
         <v>27</v>
       </c>
       <c r="F45" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H45" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2625,7 +2673,7 @@
         <v>23</v>
       </c>
       <c r="F46" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2645,10 +2693,10 @@
         <v>27</v>
       </c>
       <c r="F47" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H47" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2685,10 +2733,10 @@
         <v>27</v>
       </c>
       <c r="F49" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H49" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2708,7 +2756,7 @@
         <v>23</v>
       </c>
       <c r="F50" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2785,13 +2833,13 @@
         <v>24</v>
       </c>
       <c r="F54" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G54" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="H54" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2811,10 +2859,10 @@
         <v>27</v>
       </c>
       <c r="F55" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H55" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2888,7 +2936,7 @@
         <v>42</v>
       </c>
       <c r="F59" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2908,7 +2956,7 @@
         <v>42</v>
       </c>
       <c r="F60" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2965,13 +3013,13 @@
         <v>24</v>
       </c>
       <c r="F63" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G63" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="H63" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2991,10 +3039,10 @@
         <v>45</v>
       </c>
       <c r="H64" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="I64" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -3014,10 +3062,10 @@
         <v>46</v>
       </c>
       <c r="H65" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="I65" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -3054,7 +3102,7 @@
         <v>27</v>
       </c>
       <c r="F67" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -3074,13 +3122,13 @@
         <v>47</v>
       </c>
       <c r="F68" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="H68" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="I68" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -3100,13 +3148,13 @@
         <v>23</v>
       </c>
       <c r="F69" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="H69" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="I69" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -3146,10 +3194,10 @@
         <v>45</v>
       </c>
       <c r="H71" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="I71" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -3169,13 +3217,13 @@
         <v>48</v>
       </c>
       <c r="F72" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="H72" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="I72" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -3195,13 +3243,13 @@
         <v>48</v>
       </c>
       <c r="F73" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="H73" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="I73" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -3221,7 +3269,7 @@
         <v>23</v>
       </c>
       <c r="F74" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -3241,10 +3289,10 @@
         <v>49</v>
       </c>
       <c r="H75" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="I75" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -3264,10 +3312,10 @@
         <v>50</v>
       </c>
       <c r="H76" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="I76" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -3287,10 +3335,10 @@
         <v>51</v>
       </c>
       <c r="H77" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="I77" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -3327,10 +3375,10 @@
         <v>53</v>
       </c>
       <c r="H79" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="I79" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -3350,10 +3398,10 @@
         <v>22</v>
       </c>
       <c r="H80" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="I80" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -3376,10 +3424,10 @@
         <v>21</v>
       </c>
       <c r="H81" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="I81" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -3399,10 +3447,10 @@
         <v>54</v>
       </c>
       <c r="H82" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="I82" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3422,10 +3470,10 @@
         <v>55</v>
       </c>
       <c r="H83" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="I83" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -3445,10 +3493,10 @@
         <v>32</v>
       </c>
       <c r="H84" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I84" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -3468,10 +3516,10 @@
         <v>56</v>
       </c>
       <c r="H85" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="I85" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -3491,10 +3539,10 @@
         <v>57</v>
       </c>
       <c r="H86" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="I86" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -3517,10 +3565,10 @@
         <v>21</v>
       </c>
       <c r="H87" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="I87" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -3540,13 +3588,13 @@
         <v>23</v>
       </c>
       <c r="F88" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H88" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="I88" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -3569,10 +3617,10 @@
         <v>21</v>
       </c>
       <c r="H89" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="I89" t="s">
-        <v>408</v>
+        <v>422</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -3592,10 +3640,10 @@
         <v>59</v>
       </c>
       <c r="H90" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="I90" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3615,7 +3663,7 @@
         <v>23</v>
       </c>
       <c r="F91" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -3675,10 +3723,10 @@
         <v>21</v>
       </c>
       <c r="H94" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="I94" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -3698,13 +3746,13 @@
         <v>23</v>
       </c>
       <c r="F95" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="H95" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="I95" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -3724,13 +3772,13 @@
         <v>23</v>
       </c>
       <c r="F96" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H96" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="I96" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -3750,13 +3798,13 @@
         <v>61</v>
       </c>
       <c r="F97" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="H97" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="I97" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -3776,10 +3824,10 @@
         <v>62</v>
       </c>
       <c r="H98" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="I98" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -3799,13 +3847,13 @@
         <v>23</v>
       </c>
       <c r="F99" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H99" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="I99" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -3825,10 +3873,10 @@
         <v>55</v>
       </c>
       <c r="H100" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="I100" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -3848,7 +3896,7 @@
         <v>29</v>
       </c>
       <c r="F101" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -3868,10 +3916,10 @@
         <v>55</v>
       </c>
       <c r="H102" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="I102" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -3891,13 +3939,13 @@
         <v>63</v>
       </c>
       <c r="F103" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H103" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="I103" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -3917,13 +3965,13 @@
         <v>63</v>
       </c>
       <c r="F104" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H104" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="I104" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -3943,10 +3991,10 @@
         <v>36</v>
       </c>
       <c r="H105" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="I105" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -3966,13 +4014,13 @@
         <v>63</v>
       </c>
       <c r="F106" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="H106" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="I106" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -3992,13 +4040,13 @@
         <v>42</v>
       </c>
       <c r="F107" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="H107" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="I107" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -4018,13 +4066,13 @@
         <v>23</v>
       </c>
       <c r="F108" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H108" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="I108" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -4044,13 +4092,13 @@
         <v>23</v>
       </c>
       <c r="F109" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H109" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="I109" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -4070,10 +4118,10 @@
         <v>32</v>
       </c>
       <c r="H110" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="I110" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -4093,10 +4141,10 @@
         <v>24</v>
       </c>
       <c r="H111" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="I111" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -4116,7 +4164,7 @@
         <v>27</v>
       </c>
       <c r="F112" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="113" spans="1:9">
@@ -4136,10 +4184,10 @@
         <v>45</v>
       </c>
       <c r="H113" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="I113" t="s">
-        <v>408</v>
+        <v>422</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -4176,13 +4224,13 @@
         <v>65</v>
       </c>
       <c r="F115" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H115" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="I115" t="s">
-        <v>408</v>
+        <v>422</v>
       </c>
     </row>
     <row r="116" spans="1:9">
@@ -4218,6 +4266,9 @@
       <c r="E117" t="s">
         <v>67</v>
       </c>
+      <c r="H117" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" s="1">
@@ -4236,10 +4287,10 @@
         <v>46</v>
       </c>
       <c r="H118" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="I118" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="119" spans="1:9">
@@ -4276,10 +4327,10 @@
         <v>68</v>
       </c>
       <c r="H120" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="I120" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="121" spans="1:9">
@@ -4299,7 +4350,7 @@
         <v>23</v>
       </c>
       <c r="F121" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="122" spans="1:9">
@@ -4339,10 +4390,10 @@
         <v>21</v>
       </c>
       <c r="H123" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="I123" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="124" spans="1:9">
@@ -4362,10 +4413,10 @@
         <v>70</v>
       </c>
       <c r="H124" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="I124" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="125" spans="1:9">
@@ -4385,13 +4436,13 @@
         <v>27</v>
       </c>
       <c r="F125" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="H125" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="I125" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="126" spans="1:9">
@@ -4411,10 +4462,10 @@
         <v>36</v>
       </c>
       <c r="H126" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="I126" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="127" spans="1:9">
@@ -4451,10 +4502,10 @@
         <v>28</v>
       </c>
       <c r="H128" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="I128" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="129" spans="1:9">
@@ -4474,13 +4525,13 @@
         <v>23</v>
       </c>
       <c r="F129" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H129" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="I129" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -4500,10 +4551,10 @@
         <v>71</v>
       </c>
       <c r="H130" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="I130" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="131" spans="1:9">
@@ -4523,10 +4574,10 @@
         <v>72</v>
       </c>
       <c r="H131" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="I131" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="132" spans="1:9">
@@ -4546,13 +4597,13 @@
         <v>23</v>
       </c>
       <c r="F132" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H132" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="I132" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="133" spans="1:9">
@@ -4572,10 +4623,10 @@
         <v>27</v>
       </c>
       <c r="F133" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="H133" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
     </row>
     <row r="134" spans="1:9">
@@ -4595,7 +4646,7 @@
         <v>34</v>
       </c>
       <c r="F134" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="135" spans="1:9">
@@ -4635,10 +4686,10 @@
         <v>55</v>
       </c>
       <c r="H136" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="I136" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="137" spans="1:9">
@@ -4658,13 +4709,13 @@
         <v>73</v>
       </c>
       <c r="F137" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H137" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="I137" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="138" spans="1:9">
@@ -4684,10 +4735,10 @@
         <v>27</v>
       </c>
       <c r="F138" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H138" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="139" spans="1:9">
@@ -4707,10 +4758,10 @@
         <v>27</v>
       </c>
       <c r="F139" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H139" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="140" spans="1:9">
@@ -4730,13 +4781,13 @@
         <v>74</v>
       </c>
       <c r="F140" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H140" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="I140" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="141" spans="1:9">
@@ -4756,13 +4807,13 @@
         <v>23</v>
       </c>
       <c r="F141" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H141" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="I141" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="142" spans="1:9">
@@ -4802,10 +4853,10 @@
         <v>69</v>
       </c>
       <c r="H143" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="I143" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -4825,10 +4876,10 @@
         <v>53</v>
       </c>
       <c r="H144" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="I144" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -4848,10 +4899,10 @@
         <v>22</v>
       </c>
       <c r="H145" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="I145" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -4871,13 +4922,13 @@
         <v>23</v>
       </c>
       <c r="F146" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H146" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="I146" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -4897,10 +4948,10 @@
         <v>27</v>
       </c>
       <c r="F147" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H147" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -4920,7 +4971,10 @@
         <v>34</v>
       </c>
       <c r="F148" t="s">
-        <v>150</v>
+        <v>153</v>
+      </c>
+      <c r="H148" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -4940,7 +4994,7 @@
         <v>34</v>
       </c>
       <c r="F149" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -4960,7 +5014,7 @@
         <v>23</v>
       </c>
       <c r="F150" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -4980,13 +5034,13 @@
         <v>23</v>
       </c>
       <c r="F151" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H151" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="I151" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -5006,13 +5060,13 @@
         <v>23</v>
       </c>
       <c r="F152" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="H152" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="I152" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -5032,13 +5086,13 @@
         <v>42</v>
       </c>
       <c r="F153" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H153" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="I153" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="154" spans="1:9">
@@ -5058,7 +5112,7 @@
         <v>27</v>
       </c>
       <c r="F154" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -5078,13 +5132,13 @@
         <v>23</v>
       </c>
       <c r="F155" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="H155" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="I155" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="156" spans="1:9">
@@ -5104,10 +5158,10 @@
         <v>75</v>
       </c>
       <c r="H156" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="I156" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="157" spans="1:9">
@@ -5127,10 +5181,10 @@
         <v>76</v>
       </c>
       <c r="H157" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="I157" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="158" spans="1:9">
@@ -5167,13 +5221,13 @@
         <v>77</v>
       </c>
       <c r="F159" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H159" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="I159" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="160" spans="1:9">
@@ -5193,10 +5247,10 @@
         <v>78</v>
       </c>
       <c r="H160" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="I160" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="161" spans="1:9">
@@ -5216,13 +5270,13 @@
         <v>23</v>
       </c>
       <c r="F161" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H161" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="I161" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="162" spans="1:9">
@@ -5242,10 +5296,10 @@
         <v>79</v>
       </c>
       <c r="H162" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="I162" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="163" spans="1:9">
@@ -5265,13 +5319,13 @@
         <v>23</v>
       </c>
       <c r="F163" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H163" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="I163" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="164" spans="1:9">
@@ -5311,7 +5365,7 @@
         <v>21</v>
       </c>
       <c r="H165" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="166" spans="1:9">
@@ -5331,13 +5385,13 @@
         <v>23</v>
       </c>
       <c r="F166" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H166" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="I166" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="167" spans="1:9">
@@ -5374,13 +5428,13 @@
         <v>24</v>
       </c>
       <c r="F168" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G168" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="H168" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
     </row>
     <row r="169" spans="1:9">
@@ -5400,13 +5454,13 @@
         <v>42</v>
       </c>
       <c r="F169" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H169" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="I169" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="170" spans="1:9">
@@ -5426,10 +5480,10 @@
         <v>32</v>
       </c>
       <c r="H170" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="I170" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="171" spans="1:9">
@@ -5449,10 +5503,10 @@
         <v>46</v>
       </c>
       <c r="H171" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="I171" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="172" spans="1:9">
@@ -5472,10 +5526,10 @@
         <v>82</v>
       </c>
       <c r="H172" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="I172" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="173" spans="1:9">
@@ -5495,10 +5549,10 @@
         <v>59</v>
       </c>
       <c r="H173" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="I173" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="174" spans="1:9">
@@ -5518,13 +5572,13 @@
         <v>32</v>
       </c>
       <c r="F174" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H174" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="I174" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="175" spans="1:9">
@@ -5547,10 +5601,10 @@
         <v>21</v>
       </c>
       <c r="H175" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="I175" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="176" spans="1:9">
@@ -5570,13 +5624,13 @@
         <v>23</v>
       </c>
       <c r="F176" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H176" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="I176" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="177" spans="1:9">
@@ -5596,7 +5650,7 @@
         <v>27</v>
       </c>
       <c r="F177" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="178" spans="1:9">
@@ -5616,10 +5670,10 @@
         <v>83</v>
       </c>
       <c r="H178" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="I178" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="179" spans="1:9">
@@ -5639,10 +5693,10 @@
         <v>84</v>
       </c>
       <c r="H179" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="I179" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="180" spans="1:9">
@@ -5662,13 +5716,13 @@
         <v>42</v>
       </c>
       <c r="F180" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="H180" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="I180" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="181" spans="1:9">
@@ -5688,13 +5742,13 @@
         <v>42</v>
       </c>
       <c r="F181" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H181" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="I181" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="182" spans="1:9">
@@ -5717,10 +5771,10 @@
         <v>21</v>
       </c>
       <c r="H182" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="I182" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="183" spans="1:9">
@@ -5740,10 +5794,10 @@
         <v>24</v>
       </c>
       <c r="F183" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G183" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="184" spans="1:9">
@@ -5763,10 +5817,10 @@
         <v>85</v>
       </c>
       <c r="H184" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="I184" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="185" spans="1:9">
@@ -5786,7 +5840,7 @@
         <v>23</v>
       </c>
       <c r="F185" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="186" spans="1:9">
@@ -5806,10 +5860,10 @@
         <v>86</v>
       </c>
       <c r="H186" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="I186" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="187" spans="1:9">
@@ -5829,13 +5883,13 @@
         <v>87</v>
       </c>
       <c r="F187" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="H187" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="I187" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="188" spans="1:9">
@@ -5855,13 +5909,13 @@
         <v>23</v>
       </c>
       <c r="F188" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H188" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="I188" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="189" spans="1:9">
@@ -5881,10 +5935,10 @@
         <v>88</v>
       </c>
       <c r="H189" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="I189" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="190" spans="1:9">
@@ -5904,10 +5958,10 @@
         <v>21</v>
       </c>
       <c r="H190" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="I190" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="191" spans="1:9">
@@ -5927,10 +5981,10 @@
         <v>89</v>
       </c>
       <c r="F191" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="H191" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
     </row>
     <row r="192" spans="1:9">
@@ -5950,10 +6004,10 @@
         <v>46</v>
       </c>
       <c r="H192" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="I192" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="193" spans="1:9">
@@ -5973,10 +6027,10 @@
         <v>90</v>
       </c>
       <c r="H193" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="I193" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="194" spans="1:9">
@@ -5999,10 +6053,10 @@
         <v>21</v>
       </c>
       <c r="H194" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="I194" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="195" spans="1:9">
@@ -6022,10 +6076,10 @@
         <v>22</v>
       </c>
       <c r="H195" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="I195" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="196" spans="1:9">
@@ -6045,13 +6099,13 @@
         <v>42</v>
       </c>
       <c r="F196" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H196" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="I196" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="197" spans="1:9">
@@ -6071,13 +6125,13 @@
         <v>23</v>
       </c>
       <c r="F197" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H197" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="I197" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="198" spans="1:9">
@@ -6097,10 +6151,10 @@
         <v>55</v>
       </c>
       <c r="H198" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="I198" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="199" spans="1:9">
@@ -6120,13 +6174,13 @@
         <v>23</v>
       </c>
       <c r="F199" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H199" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="I199" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="200" spans="1:9">
@@ -6146,13 +6200,13 @@
         <v>23</v>
       </c>
       <c r="F200" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H200" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="I200" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="201" spans="1:9">
@@ -6172,13 +6226,13 @@
         <v>23</v>
       </c>
       <c r="F201" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H201" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="I201" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="202" spans="1:9">
@@ -6198,13 +6252,13 @@
         <v>91</v>
       </c>
       <c r="F202" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="H202" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="I202" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="203" spans="1:9">
@@ -6224,10 +6278,10 @@
         <v>56</v>
       </c>
       <c r="H203" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="I203" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="204" spans="1:9">
@@ -6247,10 +6301,10 @@
         <v>56</v>
       </c>
       <c r="H204" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="I204" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="205" spans="1:9">
@@ -6270,10 +6324,10 @@
         <v>55</v>
       </c>
       <c r="H205" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="I205" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="206" spans="1:9">
@@ -6293,10 +6347,10 @@
         <v>55</v>
       </c>
       <c r="H206" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="I206" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="207" spans="1:9">
@@ -6316,10 +6370,10 @@
         <v>32</v>
       </c>
       <c r="H207" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="I207" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="208" spans="1:9">
@@ -6339,7 +6393,7 @@
         <v>92</v>
       </c>
       <c r="F208" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="209" spans="1:9">
@@ -6359,10 +6413,10 @@
         <v>93</v>
       </c>
       <c r="H209" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="I209" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="210" spans="1:9">
@@ -6382,10 +6436,10 @@
         <v>36</v>
       </c>
       <c r="H210" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="I210" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="211" spans="1:9">
@@ -6405,10 +6459,10 @@
         <v>55</v>
       </c>
       <c r="H211" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="I211" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="212" spans="1:9">
@@ -6428,13 +6482,13 @@
         <v>23</v>
       </c>
       <c r="F212" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H212" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="I212" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="213" spans="1:9">
@@ -6454,13 +6508,13 @@
         <v>23</v>
       </c>
       <c r="F213" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H213" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="I213" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="214" spans="1:9">
@@ -6480,10 +6534,10 @@
         <v>55</v>
       </c>
       <c r="H214" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="I214" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="215" spans="1:9">
@@ -6503,13 +6557,13 @@
         <v>23</v>
       </c>
       <c r="F215" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H215" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="I215" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="216" spans="1:9">
@@ -6529,10 +6583,10 @@
         <v>94</v>
       </c>
       <c r="H216" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="I216" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="217" spans="1:9">
@@ -6552,13 +6606,13 @@
         <v>95</v>
       </c>
       <c r="F217" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H217" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="I217" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="218" spans="1:9">
@@ -6578,13 +6632,13 @@
         <v>23</v>
       </c>
       <c r="F218" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H218" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="I218" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="219" spans="1:9">
@@ -6604,13 +6658,13 @@
         <v>96</v>
       </c>
       <c r="F219" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H219" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="I219" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="220" spans="1:9">
@@ -6630,10 +6684,10 @@
         <v>32</v>
       </c>
       <c r="H220" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="I220" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="221" spans="1:9">
@@ -6653,13 +6707,13 @@
         <v>96</v>
       </c>
       <c r="F221" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H221" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="I221" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="222" spans="1:9">
@@ -6679,13 +6733,13 @@
         <v>23</v>
       </c>
       <c r="F222" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H222" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="I222" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="223" spans="1:9">
@@ -6705,13 +6759,13 @@
         <v>23</v>
       </c>
       <c r="F223" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H223" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="I223" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="224" spans="1:9">
@@ -6748,13 +6802,13 @@
         <v>96</v>
       </c>
       <c r="F225" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H225" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="I225" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="226" spans="1:9">
@@ -6791,13 +6845,13 @@
         <v>96</v>
       </c>
       <c r="F227" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H227" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="I227" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="228" spans="1:9">
@@ -6834,10 +6888,10 @@
         <v>99</v>
       </c>
       <c r="H229" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="I229" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="230" spans="1:9">
@@ -6857,13 +6911,13 @@
         <v>96</v>
       </c>
       <c r="F230" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H230" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="I230" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="231" spans="1:9">
@@ -6883,10 +6937,10 @@
         <v>100</v>
       </c>
       <c r="H231" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="I231" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="232" spans="1:9">
@@ -6940,10 +6994,10 @@
         <v>102</v>
       </c>
       <c r="H234" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="I234" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="235" spans="1:9">
@@ -6963,13 +7017,13 @@
         <v>103</v>
       </c>
       <c r="F235" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="H235" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="I235" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="236" spans="1:9">
@@ -6989,13 +7043,13 @@
         <v>23</v>
       </c>
       <c r="F236" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H236" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="I236" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="237" spans="1:9">
@@ -7015,10 +7069,10 @@
         <v>104</v>
       </c>
       <c r="H237" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="I237" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="238" spans="1:9">
@@ -7038,13 +7092,13 @@
         <v>23</v>
       </c>
       <c r="F238" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H238" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="I238" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="239" spans="1:9">
@@ -7064,13 +7118,13 @@
         <v>23</v>
       </c>
       <c r="F239" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H239" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="I239" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="240" spans="1:9">
@@ -7090,10 +7144,10 @@
         <v>105</v>
       </c>
       <c r="H240" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="I240" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="241" spans="1:9">
@@ -7113,10 +7167,10 @@
         <v>46</v>
       </c>
       <c r="H241" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="I241" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="242" spans="1:9">
@@ -7156,10 +7210,10 @@
         <v>59</v>
       </c>
       <c r="H243" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="I243" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="244" spans="1:9">
@@ -7179,7 +7233,7 @@
         <v>23</v>
       </c>
       <c r="F244" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="245" spans="1:9">
@@ -7199,13 +7253,13 @@
         <v>92</v>
       </c>
       <c r="F245" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H245" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="I245" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="246" spans="1:9">
@@ -7225,13 +7279,13 @@
         <v>23</v>
       </c>
       <c r="F246" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H246" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="I246" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="247" spans="1:9">
@@ -7251,10 +7305,10 @@
         <v>57</v>
       </c>
       <c r="H247" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="I247" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="248" spans="1:9">
@@ -7274,7 +7328,7 @@
         <v>42</v>
       </c>
       <c r="F248" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="249" spans="1:9">
@@ -7294,13 +7348,13 @@
         <v>23</v>
       </c>
       <c r="F249" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H249" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="I249" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="250" spans="1:9">
@@ -7340,13 +7394,13 @@
         <v>23</v>
       </c>
       <c r="F251" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H251" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="I251" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="252" spans="1:9">
@@ -7366,10 +7420,10 @@
         <v>22</v>
       </c>
       <c r="H252" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="I252" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="253" spans="1:9">
@@ -7406,10 +7460,10 @@
         <v>107</v>
       </c>
       <c r="H254" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="I254" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="255" spans="1:9">
@@ -7429,13 +7483,13 @@
         <v>23</v>
       </c>
       <c r="F255" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H255" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="I255" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="256" spans="1:9">
@@ -7455,10 +7509,10 @@
         <v>108</v>
       </c>
       <c r="H256" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="I256" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="257" spans="1:9">
@@ -7478,13 +7532,13 @@
         <v>23</v>
       </c>
       <c r="F257" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H257" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="I257" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="258" spans="1:9">
@@ -7504,13 +7558,13 @@
         <v>23</v>
       </c>
       <c r="F258" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H258" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="I258" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="259" spans="1:9">
@@ -7530,10 +7584,10 @@
         <v>109</v>
       </c>
       <c r="H259" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="I259" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="260" spans="1:9">
@@ -7553,7 +7607,7 @@
         <v>27</v>
       </c>
       <c r="F260" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="261" spans="1:9">
@@ -7573,13 +7627,13 @@
         <v>23</v>
       </c>
       <c r="F261" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H261" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="I261" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="262" spans="1:9">
@@ -7599,13 +7653,13 @@
         <v>23</v>
       </c>
       <c r="F262" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H262" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="I262" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="263" spans="1:9">
@@ -7625,10 +7679,10 @@
         <v>110</v>
       </c>
       <c r="H263" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="I263" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="264" spans="1:9">
@@ -7648,10 +7702,10 @@
         <v>32</v>
       </c>
       <c r="H264" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="I264" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="265" spans="1:9">
@@ -7671,10 +7725,10 @@
         <v>32</v>
       </c>
       <c r="H265" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="I265" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="266" spans="1:9">
@@ -7694,10 +7748,10 @@
         <v>32</v>
       </c>
       <c r="H266" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="I266" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="267" spans="1:9">
@@ -7714,16 +7768,16 @@
         <v>17</v>
       </c>
       <c r="E267" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="F267" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H267" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="I267" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="268" spans="1:9">
@@ -7743,10 +7797,10 @@
         <v>32</v>
       </c>
       <c r="H268" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="I268" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="269" spans="1:9">
@@ -7766,10 +7820,10 @@
         <v>32</v>
       </c>
       <c r="H269" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="I269" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="270" spans="1:9">
@@ -7789,10 +7843,10 @@
         <v>32</v>
       </c>
       <c r="H270" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="I270" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="271" spans="1:9">
@@ -7812,10 +7866,10 @@
         <v>32</v>
       </c>
       <c r="H271" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="I271" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="272" spans="1:9">
@@ -7835,13 +7889,13 @@
         <v>23</v>
       </c>
       <c r="F272" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H272" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="I272" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="273" spans="1:9">
@@ -7861,13 +7915,13 @@
         <v>23</v>
       </c>
       <c r="F273" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H273" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I273" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="274" spans="1:9">
@@ -7907,13 +7961,13 @@
         <v>42</v>
       </c>
       <c r="F275" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="H275" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="I275" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="276" spans="1:9">
@@ -7933,13 +7987,13 @@
         <v>23</v>
       </c>
       <c r="F276" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H276" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="I276" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="277" spans="1:9">
@@ -7959,10 +8013,10 @@
         <v>32</v>
       </c>
       <c r="H277" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="I277" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="278" spans="1:9">
@@ -7982,10 +8036,10 @@
         <v>32</v>
       </c>
       <c r="H278" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="I278" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="279" spans="1:9">
@@ -8005,10 +8059,10 @@
         <v>59</v>
       </c>
       <c r="H279" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="I279" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="280" spans="1:9">
@@ -8028,13 +8082,13 @@
         <v>23</v>
       </c>
       <c r="F280" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H280" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="I280" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="281" spans="1:9">
@@ -8054,13 +8108,13 @@
         <v>23</v>
       </c>
       <c r="F281" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H281" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="I281" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="282" spans="1:9">
@@ -8080,10 +8134,10 @@
         <v>32</v>
       </c>
       <c r="H282" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="I282" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="283" spans="1:9">
@@ -8103,13 +8157,13 @@
         <v>23</v>
       </c>
       <c r="F283" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H283" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="I283" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="284" spans="1:9">
@@ -8129,10 +8183,10 @@
         <v>32</v>
       </c>
       <c r="H284" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="I284" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="285" spans="1:9">
@@ -8152,10 +8206,10 @@
         <v>32</v>
       </c>
       <c r="H285" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="I285" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="286" spans="1:9">
@@ -8175,10 +8229,10 @@
         <v>32</v>
       </c>
       <c r="H286" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="I286" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="287" spans="1:9">
@@ -8198,10 +8252,10 @@
         <v>32</v>
       </c>
       <c r="H287" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="I287" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="288" spans="1:9">
@@ -8218,13 +8272,13 @@
         <v>20</v>
       </c>
       <c r="E288" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H288" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="I288" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="289" spans="1:9">
@@ -8241,7 +8295,7 @@
         <v>16</v>
       </c>
       <c r="E289" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="290" spans="1:9">
@@ -8261,10 +8315,10 @@
         <v>28</v>
       </c>
       <c r="H290" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="I290" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="291" spans="1:9">
@@ -8284,13 +8338,13 @@
         <v>23</v>
       </c>
       <c r="F291" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H291" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="I291" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="292" spans="1:9">
@@ -8310,13 +8364,13 @@
         <v>27</v>
       </c>
       <c r="F292" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H292" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="I292" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="293" spans="1:9">
@@ -8333,13 +8387,13 @@
         <v>20</v>
       </c>
       <c r="E293" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H293" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="I293" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="294" spans="1:9">
@@ -8359,13 +8413,13 @@
         <v>23</v>
       </c>
       <c r="F294" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H294" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="I294" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="295" spans="1:9">
@@ -8385,7 +8439,7 @@
         <v>42</v>
       </c>
       <c r="F295" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="296" spans="1:9">
@@ -8405,7 +8459,7 @@
         <v>34</v>
       </c>
       <c r="F296" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="297" spans="1:9">
@@ -8425,13 +8479,13 @@
         <v>42</v>
       </c>
       <c r="F297" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H297" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="I297" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
     </row>
     <row r="298" spans="1:9">
@@ -8448,7 +8502,197 @@
         <v>20</v>
       </c>
       <c r="E298" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="299" spans="1:9">
+      <c r="A299" s="1">
+        <v>297</v>
+      </c>
+      <c r="B299" s="2">
+        <v>42768</v>
+      </c>
+      <c r="C299" t="s">
+        <v>15</v>
+      </c>
+      <c r="D299" t="s">
+        <v>17</v>
+      </c>
+      <c r="E299" t="s">
+        <v>23</v>
+      </c>
+      <c r="H299" t="s">
+        <v>412</v>
+      </c>
+      <c r="I299" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="300" spans="1:9">
+      <c r="A300" s="1">
+        <v>298</v>
+      </c>
+      <c r="B300" s="2">
+        <v>42769</v>
+      </c>
+      <c r="C300" t="s">
+        <v>9</v>
+      </c>
+      <c r="D300" t="s">
+        <v>17</v>
+      </c>
+      <c r="E300" t="s">
+        <v>23</v>
+      </c>
+      <c r="F300" t="s">
+        <v>140</v>
+      </c>
+      <c r="H300" t="s">
+        <v>413</v>
+      </c>
+      <c r="I300" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="301" spans="1:9">
+      <c r="A301" s="1">
+        <v>299</v>
+      </c>
+      <c r="B301" s="2">
+        <v>42769</v>
+      </c>
+      <c r="C301" t="s">
+        <v>9</v>
+      </c>
+      <c r="D301" t="s">
+        <v>17</v>
+      </c>
+      <c r="E301" t="s">
+        <v>23</v>
+      </c>
+      <c r="F301" t="s">
+        <v>192</v>
+      </c>
+      <c r="H301" t="s">
+        <v>414</v>
+      </c>
+      <c r="I301" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="302" spans="1:9">
+      <c r="A302" s="1">
+        <v>300</v>
+      </c>
+      <c r="B302" s="2">
+        <v>42769</v>
+      </c>
+      <c r="C302" t="s">
+        <v>9</v>
+      </c>
+      <c r="D302" t="s">
+        <v>17</v>
+      </c>
+      <c r="E302" t="s">
         <v>115</v>
+      </c>
+      <c r="H302" t="s">
+        <v>415</v>
+      </c>
+      <c r="I302" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="303" spans="1:9">
+      <c r="A303" s="1">
+        <v>301</v>
+      </c>
+      <c r="B303" s="2">
+        <v>42773</v>
+      </c>
+      <c r="C303" t="s">
+        <v>9</v>
+      </c>
+      <c r="D303" t="s">
+        <v>17</v>
+      </c>
+      <c r="E303" t="s">
+        <v>116</v>
+      </c>
+      <c r="H303" t="s">
+        <v>416</v>
+      </c>
+      <c r="I303" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="304" spans="1:9">
+      <c r="A304" s="1">
+        <v>302</v>
+      </c>
+      <c r="B304" s="2">
+        <v>42773</v>
+      </c>
+      <c r="C304" t="s">
+        <v>9</v>
+      </c>
+      <c r="D304" t="s">
+        <v>17</v>
+      </c>
+      <c r="E304" t="s">
+        <v>55</v>
+      </c>
+      <c r="H304" t="s">
+        <v>417</v>
+      </c>
+      <c r="I304" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="305" spans="1:9">
+      <c r="A305" s="1">
+        <v>303</v>
+      </c>
+      <c r="B305" s="2">
+        <v>42774</v>
+      </c>
+      <c r="C305" t="s">
+        <v>9</v>
+      </c>
+      <c r="D305" t="s">
+        <v>20</v>
+      </c>
+      <c r="E305" t="s">
+        <v>117</v>
+      </c>
+      <c r="H305" t="s">
+        <v>418</v>
+      </c>
+      <c r="I305" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="306" spans="1:9">
+      <c r="A306" s="1">
+        <v>304</v>
+      </c>
+      <c r="B306" s="2">
+        <v>42774</v>
+      </c>
+      <c r="C306" t="s">
+        <v>9</v>
+      </c>
+      <c r="D306" t="s">
+        <v>16</v>
+      </c>
+      <c r="E306" t="s">
+        <v>118</v>
+      </c>
+      <c r="H306" t="s">
+        <v>419</v>
+      </c>
+      <c r="I306" t="s">
+        <v>420</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to plotly scripts and input files
</commit_message>
<xml_diff>
--- a/xlsx/OTP_feedback_tracking_cleaned_no_pi.xlsx
+++ b/xlsx/OTP_feedback_tracking_cleaned_no_pi.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="453">
   <si>
     <t>Date Received</t>
   </si>
@@ -370,6 +370,24 @@
     <t>Would like compass on maps</t>
   </si>
   <si>
+    <t>"just wanted to say how quick and simple the process for finding available Max from Milwaukie was. I love having this option for going downtown."</t>
+  </si>
+  <si>
+    <t>Preferred previous trip planner form</t>
+  </si>
+  <si>
+    <t>Dislikes trip planner</t>
+  </si>
+  <si>
+    <t>"I Happy Nice the information as very help in any questions use in line Thank You"</t>
+  </si>
+  <si>
+    <t>"Your site is so easy to use, and informative. Thanks for making my trips so effortless."</t>
+  </si>
+  <si>
+    <t>Would like "Turn left" and "Turn rigth" directions</t>
+  </si>
+  <si>
     <t>Location outside district</t>
   </si>
   <si>
@@ -592,6 +610,15 @@
     <t>Scheduling issue; No weekend service on desired route</t>
   </si>
   <si>
+    <t>New address in latest MAF but not yet in TriMet geocoder</t>
+  </si>
+  <si>
+    <t>Wrong "Travel preference" option</t>
+  </si>
+  <si>
+    <t>User and GIS team can't replicate</t>
+  </si>
+  <si>
     <t>Vancouver</t>
   </si>
   <si>
@@ -1271,6 +1298,72 @@
   </si>
   <si>
     <t>https://trimet.org/#/planner/results/itin_num=1&amp;from=Amtrak</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#planner/results/from=Current+Location%3A%3A45.554429999999996%2C-122.68716670510707&amp;to=Kaiser+-+Mt+Scott+Medical+Office%2C+Clackamas%3A%3A45.43275%2C-122.56268&amp;mode=RAIL%2CTRAM%2CSUBWAY%2CFUNICULAR%2CGONDOLA%2CWALK&amp;m=am&amp;walk=1260&amp;arr=A</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=Milwaukie%2C+Milwaukie%3A%3A45.4416%2C-122.640396&amp;to=310+SW+Lincoln+Ave%2C+Portland</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#/planner/results/itin_num=3&amp;from=595</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=Washington+County+Fairgrounds%2C+Washington+Co.&amp;to=Providence+Park+MAX+Station+E%2C+Portland+(Stop+ID+9758)%3A%3A45.52132%2C-122.68989&amp;m=pm&amp;walk=1260&amp;arr=A</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=1100+SE+DIVISION+ST%2C+Portland%3A%3A45.50464%2C-122.654434&amp;to=Oregon+Museum+of+Science+and+Industry%2C+Portland%3A%3A45.508327%2C-122.66501&amp;m=am&amp;walk=1260&amp;arr=D</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#planner/results/from=128+NW+11TH+AVE%2C+Portland&amp;to=4506+SE+CESAR+E+CHAVEZ+BLVD%2C+Portland%3A%3A45.49003%2C-122.62249&amp;mode=RAIL%2CTRAM%2CSUBWAY%2CFUNICULAR%2CGONDOLA%2CWALK&amp;m=pm&amp;walk=1260&amp;arr=D</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/a=1&amp;arr=D&amp;from=Beaverton+Transit+Center%2C+Beaverton%3A%3A45.491085%2C-122.80114&amp;m=pm&amp;geo_type=tolist&amp;walk=1260&amp;_=1487021083116&amp;has_geocode=true&amp;to=MARK+O+HATFIELD+US+COURTHOUSE%3A%3A45.516252%2C-122.676635%3A%3APortland</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#planner/results/from=5305+SE+34TH+AVE%2C+Portland%3A%3A45.484535%2C-122.62972&amp;to=3249+SE+DIVISION+ST%2C+Portland%3A%3A45.505016%2C-122.6315&amp;m=pm&amp;walk=840&amp;arr=A</t>
+  </si>
+  <si>
+    <t>http://trimet.org/ride/stop_select_geocode.html?place=PDX%20airport</t>
+  </si>
+  <si>
+    <t>http://trimet.org/ride/planner_geocode.html?geo_type=from&amp;from=0650%20SW%20Lowell%20St.%2C%20Portland%2C%20OR%2097239</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=16982+SE+ANKENY+ST%2C+Portland%3A%3A45.521065%2C-122.48813&amp;to=20078+NE+SANDY+BLVD%2C+Fairview%3A%3A45.543385%2C-122.45782&amp;m=am&amp;walk=1260&amp;arr=A</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=6404+SE+23RD+AVE%2C+Portland%3A%3A45.476894%2C-122.64197&amp;to=1461+N+Skidmore+St+Portland+OR+97217&amp;m=pm&amp;walk=160&amp;arr=A</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=Union+Station%2FNW+5th+%26+Glisan+MAX+Stn+S%2C+Portland+(Stop+ID+7601)%3A%3A45.526733%2C-122.675606&amp;to=Portland+International+Airport+MAX+Station%2C+Portland%3A%3A45.587738%2C-122.59321</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#planner/results/from=121+sw+taylor+st%2C+portland&amp;to=220+NW+2nd+Ave%2C+Portland%2C+OR+97209&amp;m=am&amp;walk=840&amp;optimize=TRANSFERS&amp;arr=A</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=SW+Lombard+%26+Allen+-+Stop+ID+3455%3A%3A45.47699%2C-122.800202&amp;to=1736+SW+ALDER+ST%3A%3A45.52264%2C-122.689117&amp;m=pm&amp;walk=1260&amp;arr=E</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=114+NE+65TH+AVE%3A%3A45.523703%2C-122.597128&amp;to=KAISER+CLINIC+-+INTERSTATE+EAST%3A%3A45.547963%2C-122.679864%3A%3APortland&amp;m=pm&amp;walk=1609&amp;optimize=TRANSFERS&amp;arr=D</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=Merlo+Rd%2FSW+158th+Ave+MAX+Station%2C+Beaverton%3A%3A45.50523%2C-122.84215&amp;to=PDX%2C+Portland%3A%3A45.58918%2C-122.59346&amp;m=am&amp;walk=1260&amp;arr=A</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=Current+Location%3A%3A45.602432526690514%2C-122.43013313982861&amp;to=2124+N+KILLINGSWORTH+ST%2C+Portland%3A%3A45.562492%2C-122.68938</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#planner/results/from=Sunset+Transit+Center&amp;to=Casey+Eye+Institute+-+South+Waterfront%2C+Portland%3A%3A45.49881%2C-122.671165&amp;mode=RAIL%2CTRAM%2CSUBWAY%2CFUNICULAR%2CGONDOLA%2CWALK&amp;m=pm&amp;walk=1260&amp;arr=A</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=9360+SW+BEAVERTON+HILLSDALE+HWY%2C+Beaverton%3A%3A45.484272%2C-122.77298&amp;to=14600+NW+CORNELL+RD%2C+Portland%3A%3A45.530437%2C-122.82666&amp;m=pm&amp;walk=1609&amp;arr=None</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#planner/results/from=7509+NE+MASON+ST%2C+Portland%3A%3A45.552593%2C-122.58545&amp;to=13631+SE+JOHNSON+RD%2C+Milwaukie%3A%3A45.4245%2C-122.584816&amp;m=am&amp;walk=840&amp;arr=A</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=6600+N+BOSTON+AVE%2C+Portland%3A%3A45.570885%2C-122.69117&amp;to=Pioneer+Square+South+MAX+Station+E%2C+Portland+(Stop+ID+8334)%3A%3A45.518497%2C-122.679146&amp;m=am&amp;walk=1260&amp;arr=A</t>
   </si>
   <si>
     <t>Weekday</t>
@@ -1641,7 +1734,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I306"/>
+  <dimension ref="A1:I328"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1737,13 +1830,13 @@
         <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G4" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="H4" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1763,13 +1856,13 @@
         <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G5" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="H5" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1789,10 +1882,10 @@
         <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="I6" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1852,7 +1945,7 @@
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1872,13 +1965,13 @@
         <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G10" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="H10" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1915,13 +2008,13 @@
         <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G12" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="H12" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1941,7 +2034,7 @@
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1961,7 +2054,7 @@
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2001,13 +2094,13 @@
         <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G16" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="H16" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2044,7 +2137,7 @@
         <v>22</v>
       </c>
       <c r="F18" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2064,10 +2157,10 @@
         <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="H19" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2087,13 +2180,13 @@
         <v>23</v>
       </c>
       <c r="F20" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G20" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="H20" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2113,10 +2206,10 @@
         <v>26</v>
       </c>
       <c r="F21" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="H21" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2136,13 +2229,13 @@
         <v>23</v>
       </c>
       <c r="F22" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G22" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="H22" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2162,13 +2255,13 @@
         <v>23</v>
       </c>
       <c r="F23" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G23" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="H23" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2188,7 +2281,7 @@
         <v>22</v>
       </c>
       <c r="F24" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2225,7 +2318,7 @@
         <v>33</v>
       </c>
       <c r="F26" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2245,10 +2338,10 @@
         <v>26</v>
       </c>
       <c r="F27" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="H27" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2268,10 +2361,10 @@
         <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="H28" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2291,13 +2384,13 @@
         <v>23</v>
       </c>
       <c r="F29" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G29" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="H29" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2317,13 +2410,13 @@
         <v>23</v>
       </c>
       <c r="F30" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G30" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="H30" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2360,13 +2453,13 @@
         <v>23</v>
       </c>
       <c r="F32" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G32" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="H32" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2386,10 +2479,10 @@
         <v>26</v>
       </c>
       <c r="F33" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="H33" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2426,10 +2519,10 @@
         <v>23</v>
       </c>
       <c r="F35" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G35" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2449,10 +2542,10 @@
         <v>23</v>
       </c>
       <c r="F36" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G36" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2472,10 +2565,10 @@
         <v>26</v>
       </c>
       <c r="F37" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="H37" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2529,10 +2622,10 @@
         <v>26</v>
       </c>
       <c r="F40" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="H40" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2552,13 +2645,13 @@
         <v>23</v>
       </c>
       <c r="F41" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G41" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="H41" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2578,13 +2671,13 @@
         <v>23</v>
       </c>
       <c r="F42" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G42" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="H42" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2604,7 +2697,7 @@
         <v>37</v>
       </c>
       <c r="F43" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2624,10 +2717,10 @@
         <v>26</v>
       </c>
       <c r="F44" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="H44" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2647,10 +2740,10 @@
         <v>26</v>
       </c>
       <c r="F45" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="H45" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2670,7 +2763,7 @@
         <v>22</v>
       </c>
       <c r="F46" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2690,10 +2783,10 @@
         <v>26</v>
       </c>
       <c r="F47" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="H47" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2730,10 +2823,10 @@
         <v>26</v>
       </c>
       <c r="F49" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H49" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2753,7 +2846,7 @@
         <v>22</v>
       </c>
       <c r="F50" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2830,13 +2923,13 @@
         <v>23</v>
       </c>
       <c r="F54" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G54" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="H54" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2856,10 +2949,10 @@
         <v>26</v>
       </c>
       <c r="F55" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="H55" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2933,7 +3026,7 @@
         <v>41</v>
       </c>
       <c r="F59" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2953,7 +3046,7 @@
         <v>41</v>
       </c>
       <c r="F60" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -3010,13 +3103,13 @@
         <v>23</v>
       </c>
       <c r="F63" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G63" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="H63" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -3036,10 +3129,10 @@
         <v>44</v>
       </c>
       <c r="H64" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="I64" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -3059,10 +3152,10 @@
         <v>45</v>
       </c>
       <c r="H65" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="I65" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -3099,7 +3192,7 @@
         <v>26</v>
       </c>
       <c r="F67" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -3119,13 +3212,13 @@
         <v>46</v>
       </c>
       <c r="F68" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="H68" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="I68" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -3145,13 +3238,13 @@
         <v>22</v>
       </c>
       <c r="F69" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="H69" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="I69" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -3191,10 +3284,10 @@
         <v>44</v>
       </c>
       <c r="H71" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="I71" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -3214,13 +3307,13 @@
         <v>47</v>
       </c>
       <c r="F72" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="H72" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="I72" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -3240,13 +3333,13 @@
         <v>47</v>
       </c>
       <c r="F73" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="H73" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="I73" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -3266,7 +3359,7 @@
         <v>22</v>
       </c>
       <c r="F74" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -3286,10 +3379,10 @@
         <v>48</v>
       </c>
       <c r="H75" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="I75" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -3309,10 +3402,10 @@
         <v>49</v>
       </c>
       <c r="H76" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="I76" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -3332,10 +3425,10 @@
         <v>50</v>
       </c>
       <c r="H77" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="I77" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -3372,10 +3465,10 @@
         <v>52</v>
       </c>
       <c r="H79" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="I79" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -3395,10 +3488,10 @@
         <v>21</v>
       </c>
       <c r="H80" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="I80" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -3421,10 +3514,10 @@
         <v>20</v>
       </c>
       <c r="H81" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="I81" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -3444,10 +3537,10 @@
         <v>53</v>
       </c>
       <c r="H82" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="I82" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3467,10 +3560,10 @@
         <v>54</v>
       </c>
       <c r="H83" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="I83" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -3490,10 +3583,10 @@
         <v>31</v>
       </c>
       <c r="H84" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="I84" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -3513,10 +3606,10 @@
         <v>55</v>
       </c>
       <c r="H85" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="I85" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -3536,10 +3629,10 @@
         <v>56</v>
       </c>
       <c r="H86" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="I86" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -3562,10 +3655,10 @@
         <v>20</v>
       </c>
       <c r="H87" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="I87" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -3585,13 +3678,13 @@
         <v>22</v>
       </c>
       <c r="F88" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H88" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="I88" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -3614,10 +3707,10 @@
         <v>20</v>
       </c>
       <c r="H89" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="I89" t="s">
-        <v>421</v>
+        <v>452</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -3637,10 +3730,10 @@
         <v>58</v>
       </c>
       <c r="H90" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="I90" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3660,7 +3753,7 @@
         <v>22</v>
       </c>
       <c r="F91" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -3720,10 +3813,10 @@
         <v>20</v>
       </c>
       <c r="H94" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="I94" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -3743,13 +3836,13 @@
         <v>22</v>
       </c>
       <c r="F95" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="H95" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="I95" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -3769,13 +3862,13 @@
         <v>22</v>
       </c>
       <c r="F96" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="H96" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="I96" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -3795,13 +3888,13 @@
         <v>60</v>
       </c>
       <c r="F97" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="H97" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="I97" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -3821,10 +3914,10 @@
         <v>61</v>
       </c>
       <c r="H98" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="I98" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -3844,13 +3937,13 @@
         <v>22</v>
       </c>
       <c r="F99" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H99" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="I99" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -3870,10 +3963,10 @@
         <v>54</v>
       </c>
       <c r="H100" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="I100" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -3893,7 +3986,7 @@
         <v>28</v>
       </c>
       <c r="F101" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -3913,10 +4006,10 @@
         <v>54</v>
       </c>
       <c r="H102" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="I102" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -3936,13 +4029,13 @@
         <v>62</v>
       </c>
       <c r="F103" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="H103" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="I103" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -3962,13 +4055,13 @@
         <v>62</v>
       </c>
       <c r="F104" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="H104" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="I104" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -3988,10 +4081,10 @@
         <v>35</v>
       </c>
       <c r="H105" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="I105" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -4011,13 +4104,13 @@
         <v>62</v>
       </c>
       <c r="F106" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="H106" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="I106" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -4037,13 +4130,13 @@
         <v>41</v>
       </c>
       <c r="F107" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="H107" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="I107" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -4063,13 +4156,13 @@
         <v>22</v>
       </c>
       <c r="F108" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H108" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="I108" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -4089,13 +4182,13 @@
         <v>22</v>
       </c>
       <c r="F109" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="H109" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="I109" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -4115,10 +4208,10 @@
         <v>31</v>
       </c>
       <c r="H110" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="I110" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -4138,10 +4231,10 @@
         <v>23</v>
       </c>
       <c r="H111" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="I111" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -4161,7 +4254,7 @@
         <v>26</v>
       </c>
       <c r="F112" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="113" spans="1:9">
@@ -4181,10 +4274,10 @@
         <v>44</v>
       </c>
       <c r="H113" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="I113" t="s">
-        <v>421</v>
+        <v>452</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -4221,13 +4314,13 @@
         <v>64</v>
       </c>
       <c r="F115" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="H115" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="I115" t="s">
-        <v>421</v>
+        <v>452</v>
       </c>
     </row>
     <row r="116" spans="1:9">
@@ -4264,7 +4357,7 @@
         <v>66</v>
       </c>
       <c r="H117" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
     </row>
     <row r="118" spans="1:9">
@@ -4284,10 +4377,10 @@
         <v>45</v>
       </c>
       <c r="H118" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="I118" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="119" spans="1:9">
@@ -4324,10 +4417,10 @@
         <v>67</v>
       </c>
       <c r="H120" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="I120" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="121" spans="1:9">
@@ -4347,7 +4440,7 @@
         <v>22</v>
       </c>
       <c r="F121" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="122" spans="1:9">
@@ -4387,10 +4480,10 @@
         <v>20</v>
       </c>
       <c r="H123" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="I123" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="124" spans="1:9">
@@ -4410,10 +4503,10 @@
         <v>69</v>
       </c>
       <c r="H124" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="I124" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="125" spans="1:9">
@@ -4433,13 +4526,13 @@
         <v>26</v>
       </c>
       <c r="F125" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="H125" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="I125" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="126" spans="1:9">
@@ -4459,10 +4552,10 @@
         <v>35</v>
       </c>
       <c r="H126" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="I126" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="127" spans="1:9">
@@ -4499,10 +4592,10 @@
         <v>27</v>
       </c>
       <c r="H128" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="I128" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="129" spans="1:9">
@@ -4522,13 +4615,13 @@
         <v>22</v>
       </c>
       <c r="F129" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="H129" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="I129" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -4548,10 +4641,10 @@
         <v>70</v>
       </c>
       <c r="H130" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="I130" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="131" spans="1:9">
@@ -4571,10 +4664,10 @@
         <v>71</v>
       </c>
       <c r="H131" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="I131" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="132" spans="1:9">
@@ -4594,13 +4687,13 @@
         <v>22</v>
       </c>
       <c r="F132" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="H132" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="I132" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="133" spans="1:9">
@@ -4620,10 +4713,10 @@
         <v>26</v>
       </c>
       <c r="F133" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="H133" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
     </row>
     <row r="134" spans="1:9">
@@ -4643,7 +4736,7 @@
         <v>33</v>
       </c>
       <c r="F134" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="135" spans="1:9">
@@ -4683,10 +4776,10 @@
         <v>54</v>
       </c>
       <c r="H136" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="I136" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="137" spans="1:9">
@@ -4706,13 +4799,13 @@
         <v>72</v>
       </c>
       <c r="F137" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="H137" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="I137" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="138" spans="1:9">
@@ -4732,10 +4825,10 @@
         <v>26</v>
       </c>
       <c r="F138" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="H138" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
     </row>
     <row r="139" spans="1:9">
@@ -4755,10 +4848,10 @@
         <v>26</v>
       </c>
       <c r="F139" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="H139" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
     </row>
     <row r="140" spans="1:9">
@@ -4778,13 +4871,13 @@
         <v>73</v>
       </c>
       <c r="F140" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H140" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="I140" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="141" spans="1:9">
@@ -4804,13 +4897,13 @@
         <v>22</v>
       </c>
       <c r="F141" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H141" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="I141" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="142" spans="1:9">
@@ -4850,10 +4943,10 @@
         <v>68</v>
       </c>
       <c r="H143" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="I143" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -4873,10 +4966,10 @@
         <v>52</v>
       </c>
       <c r="H144" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="I144" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -4896,10 +4989,10 @@
         <v>21</v>
       </c>
       <c r="H145" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="I145" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -4919,13 +5012,13 @@
         <v>22</v>
       </c>
       <c r="F146" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="H146" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="I146" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -4945,10 +5038,10 @@
         <v>26</v>
       </c>
       <c r="F147" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="H147" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -4968,10 +5061,10 @@
         <v>33</v>
       </c>
       <c r="F148" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="H148" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -4991,7 +5084,7 @@
         <v>33</v>
       </c>
       <c r="F149" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -5011,7 +5104,7 @@
         <v>22</v>
       </c>
       <c r="F150" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -5031,13 +5124,13 @@
         <v>22</v>
       </c>
       <c r="F151" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H151" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="I151" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -5057,13 +5150,13 @@
         <v>22</v>
       </c>
       <c r="F152" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="H152" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="I152" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -5083,13 +5176,13 @@
         <v>41</v>
       </c>
       <c r="F153" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="H153" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="I153" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="154" spans="1:9">
@@ -5109,7 +5202,7 @@
         <v>26</v>
       </c>
       <c r="F154" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -5129,13 +5222,13 @@
         <v>22</v>
       </c>
       <c r="F155" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="H155" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="I155" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="156" spans="1:9">
@@ -5155,10 +5248,10 @@
         <v>74</v>
       </c>
       <c r="H156" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="I156" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="157" spans="1:9">
@@ -5178,10 +5271,10 @@
         <v>75</v>
       </c>
       <c r="H157" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="I157" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="158" spans="1:9">
@@ -5218,13 +5311,13 @@
         <v>76</v>
       </c>
       <c r="F159" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="H159" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="I159" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="160" spans="1:9">
@@ -5244,10 +5337,10 @@
         <v>77</v>
       </c>
       <c r="H160" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="I160" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="161" spans="1:9">
@@ -5267,13 +5360,13 @@
         <v>22</v>
       </c>
       <c r="F161" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H161" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="I161" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="162" spans="1:9">
@@ -5293,10 +5386,10 @@
         <v>78</v>
       </c>
       <c r="H162" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="I162" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="163" spans="1:9">
@@ -5316,13 +5409,13 @@
         <v>22</v>
       </c>
       <c r="F163" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="H163" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="I163" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="164" spans="1:9">
@@ -5362,7 +5455,7 @@
         <v>20</v>
       </c>
       <c r="H165" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
     </row>
     <row r="166" spans="1:9">
@@ -5382,13 +5475,13 @@
         <v>22</v>
       </c>
       <c r="F166" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H166" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="I166" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="167" spans="1:9">
@@ -5425,13 +5518,13 @@
         <v>23</v>
       </c>
       <c r="F168" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G168" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="H168" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
     </row>
     <row r="169" spans="1:9">
@@ -5451,13 +5544,13 @@
         <v>41</v>
       </c>
       <c r="F169" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="H169" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="I169" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="170" spans="1:9">
@@ -5477,10 +5570,10 @@
         <v>31</v>
       </c>
       <c r="H170" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="I170" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="171" spans="1:9">
@@ -5500,10 +5593,10 @@
         <v>45</v>
       </c>
       <c r="H171" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="I171" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="172" spans="1:9">
@@ -5523,10 +5616,10 @@
         <v>81</v>
       </c>
       <c r="H172" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="I172" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="173" spans="1:9">
@@ -5546,10 +5639,10 @@
         <v>58</v>
       </c>
       <c r="H173" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="I173" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="174" spans="1:9">
@@ -5569,13 +5662,13 @@
         <v>31</v>
       </c>
       <c r="F174" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="H174" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="I174" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="175" spans="1:9">
@@ -5598,10 +5691,10 @@
         <v>20</v>
       </c>
       <c r="H175" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="I175" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="176" spans="1:9">
@@ -5621,13 +5714,13 @@
         <v>22</v>
       </c>
       <c r="F176" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="H176" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="I176" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="177" spans="1:9">
@@ -5647,7 +5740,7 @@
         <v>26</v>
       </c>
       <c r="F177" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="178" spans="1:9">
@@ -5667,10 +5760,10 @@
         <v>82</v>
       </c>
       <c r="H178" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="I178" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="179" spans="1:9">
@@ -5690,10 +5783,10 @@
         <v>83</v>
       </c>
       <c r="H179" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="I179" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="180" spans="1:9">
@@ -5713,13 +5806,13 @@
         <v>41</v>
       </c>
       <c r="F180" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="H180" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="I180" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="181" spans="1:9">
@@ -5739,13 +5832,13 @@
         <v>41</v>
       </c>
       <c r="F181" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="H181" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="I181" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="182" spans="1:9">
@@ -5768,10 +5861,10 @@
         <v>20</v>
       </c>
       <c r="H182" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="I182" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="183" spans="1:9">
@@ -5791,10 +5884,10 @@
         <v>23</v>
       </c>
       <c r="F183" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G183" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="184" spans="1:9">
@@ -5814,10 +5907,10 @@
         <v>84</v>
       </c>
       <c r="H184" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="I184" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="185" spans="1:9">
@@ -5837,7 +5930,7 @@
         <v>22</v>
       </c>
       <c r="F185" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="186" spans="1:9">
@@ -5857,10 +5950,10 @@
         <v>85</v>
       </c>
       <c r="H186" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="I186" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="187" spans="1:9">
@@ -5880,13 +5973,13 @@
         <v>86</v>
       </c>
       <c r="F187" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="H187" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="I187" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="188" spans="1:9">
@@ -5906,13 +5999,13 @@
         <v>22</v>
       </c>
       <c r="F188" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="H188" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="I188" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="189" spans="1:9">
@@ -5932,10 +6025,10 @@
         <v>87</v>
       </c>
       <c r="H189" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="I189" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="190" spans="1:9">
@@ -5955,10 +6048,10 @@
         <v>20</v>
       </c>
       <c r="H190" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="I190" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="191" spans="1:9">
@@ -5978,10 +6071,10 @@
         <v>88</v>
       </c>
       <c r="F191" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="H191" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
     </row>
     <row r="192" spans="1:9">
@@ -6001,10 +6094,10 @@
         <v>45</v>
       </c>
       <c r="H192" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="I192" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="193" spans="1:9">
@@ -6024,10 +6117,10 @@
         <v>89</v>
       </c>
       <c r="H193" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="I193" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="194" spans="1:9">
@@ -6050,10 +6143,10 @@
         <v>20</v>
       </c>
       <c r="H194" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="I194" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="195" spans="1:9">
@@ -6073,10 +6166,10 @@
         <v>21</v>
       </c>
       <c r="H195" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="I195" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="196" spans="1:9">
@@ -6096,13 +6189,13 @@
         <v>41</v>
       </c>
       <c r="F196" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="H196" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="I196" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="197" spans="1:9">
@@ -6122,13 +6215,13 @@
         <v>22</v>
       </c>
       <c r="F197" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H197" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="I197" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="198" spans="1:9">
@@ -6148,10 +6241,10 @@
         <v>54</v>
       </c>
       <c r="H198" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="I198" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="199" spans="1:9">
@@ -6171,13 +6264,13 @@
         <v>22</v>
       </c>
       <c r="F199" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="H199" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="I199" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="200" spans="1:9">
@@ -6197,13 +6290,13 @@
         <v>22</v>
       </c>
       <c r="F200" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="H200" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="I200" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="201" spans="1:9">
@@ -6223,13 +6316,13 @@
         <v>22</v>
       </c>
       <c r="F201" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="H201" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="I201" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="202" spans="1:9">
@@ -6249,13 +6342,13 @@
         <v>90</v>
       </c>
       <c r="F202" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="H202" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="I202" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="203" spans="1:9">
@@ -6275,10 +6368,10 @@
         <v>55</v>
       </c>
       <c r="H203" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="I203" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="204" spans="1:9">
@@ -6298,10 +6391,10 @@
         <v>55</v>
       </c>
       <c r="H204" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="I204" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="205" spans="1:9">
@@ -6321,10 +6414,10 @@
         <v>54</v>
       </c>
       <c r="H205" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="I205" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="206" spans="1:9">
@@ -6344,10 +6437,10 @@
         <v>54</v>
       </c>
       <c r="H206" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="I206" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="207" spans="1:9">
@@ -6367,10 +6460,10 @@
         <v>31</v>
       </c>
       <c r="H207" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="I207" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="208" spans="1:9">
@@ -6390,7 +6483,7 @@
         <v>91</v>
       </c>
       <c r="F208" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="209" spans="1:9">
@@ -6410,10 +6503,10 @@
         <v>92</v>
       </c>
       <c r="H209" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="I209" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="210" spans="1:9">
@@ -6433,10 +6526,10 @@
         <v>35</v>
       </c>
       <c r="H210" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="I210" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="211" spans="1:9">
@@ -6456,10 +6549,10 @@
         <v>54</v>
       </c>
       <c r="H211" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="I211" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="212" spans="1:9">
@@ -6479,13 +6572,13 @@
         <v>22</v>
       </c>
       <c r="F212" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="H212" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="I212" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="213" spans="1:9">
@@ -6505,13 +6598,13 @@
         <v>22</v>
       </c>
       <c r="F213" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="H213" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="I213" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="214" spans="1:9">
@@ -6531,10 +6624,10 @@
         <v>54</v>
       </c>
       <c r="H214" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="I214" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="215" spans="1:9">
@@ -6554,13 +6647,13 @@
         <v>22</v>
       </c>
       <c r="F215" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H215" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="I215" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="216" spans="1:9">
@@ -6580,10 +6673,10 @@
         <v>93</v>
       </c>
       <c r="H216" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="I216" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="217" spans="1:9">
@@ -6603,13 +6696,13 @@
         <v>94</v>
       </c>
       <c r="F217" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="H217" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="I217" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="218" spans="1:9">
@@ -6629,13 +6722,13 @@
         <v>22</v>
       </c>
       <c r="F218" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H218" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="I218" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="219" spans="1:9">
@@ -6655,13 +6748,13 @@
         <v>95</v>
       </c>
       <c r="F219" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="H219" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="I219" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="220" spans="1:9">
@@ -6681,10 +6774,10 @@
         <v>31</v>
       </c>
       <c r="H220" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="I220" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="221" spans="1:9">
@@ -6704,13 +6797,13 @@
         <v>95</v>
       </c>
       <c r="F221" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="H221" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="I221" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="222" spans="1:9">
@@ -6730,13 +6823,13 @@
         <v>22</v>
       </c>
       <c r="F222" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H222" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="I222" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="223" spans="1:9">
@@ -6756,13 +6849,13 @@
         <v>22</v>
       </c>
       <c r="F223" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H223" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="I223" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="224" spans="1:9">
@@ -6799,13 +6892,13 @@
         <v>95</v>
       </c>
       <c r="F225" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="H225" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="I225" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="226" spans="1:9">
@@ -6842,13 +6935,13 @@
         <v>95</v>
       </c>
       <c r="F227" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="H227" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="I227" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="228" spans="1:9">
@@ -6885,10 +6978,10 @@
         <v>98</v>
       </c>
       <c r="H229" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="I229" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="230" spans="1:9">
@@ -6908,13 +7001,13 @@
         <v>95</v>
       </c>
       <c r="F230" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="H230" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="I230" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="231" spans="1:9">
@@ -6934,10 +7027,10 @@
         <v>99</v>
       </c>
       <c r="H231" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="I231" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="232" spans="1:9">
@@ -6991,10 +7084,10 @@
         <v>101</v>
       </c>
       <c r="H234" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="I234" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="235" spans="1:9">
@@ -7014,13 +7107,13 @@
         <v>102</v>
       </c>
       <c r="F235" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="H235" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="I235" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="236" spans="1:9">
@@ -7040,13 +7133,13 @@
         <v>22</v>
       </c>
       <c r="F236" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H236" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="I236" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="237" spans="1:9">
@@ -7066,10 +7159,10 @@
         <v>103</v>
       </c>
       <c r="H237" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="I237" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="238" spans="1:9">
@@ -7089,13 +7182,13 @@
         <v>22</v>
       </c>
       <c r="F238" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H238" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="I238" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="239" spans="1:9">
@@ -7115,13 +7208,13 @@
         <v>22</v>
       </c>
       <c r="F239" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H239" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="I239" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="240" spans="1:9">
@@ -7141,10 +7234,10 @@
         <v>104</v>
       </c>
       <c r="H240" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="I240" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="241" spans="1:9">
@@ -7164,10 +7257,10 @@
         <v>45</v>
       </c>
       <c r="H241" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
       <c r="I241" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="242" spans="1:9">
@@ -7207,10 +7300,10 @@
         <v>58</v>
       </c>
       <c r="H243" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="I243" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="244" spans="1:9">
@@ -7230,7 +7323,7 @@
         <v>22</v>
       </c>
       <c r="F244" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="245" spans="1:9">
@@ -7250,13 +7343,13 @@
         <v>91</v>
       </c>
       <c r="F245" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="H245" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="I245" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="246" spans="1:9">
@@ -7276,13 +7369,13 @@
         <v>22</v>
       </c>
       <c r="F246" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="H246" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="I246" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="247" spans="1:9">
@@ -7302,10 +7395,10 @@
         <v>56</v>
       </c>
       <c r="H247" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="I247" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="248" spans="1:9">
@@ -7325,7 +7418,7 @@
         <v>41</v>
       </c>
       <c r="F248" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="249" spans="1:9">
@@ -7345,13 +7438,13 @@
         <v>22</v>
       </c>
       <c r="F249" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H249" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="I249" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="250" spans="1:9">
@@ -7391,13 +7484,13 @@
         <v>22</v>
       </c>
       <c r="F251" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="H251" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="I251" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="252" spans="1:9">
@@ -7417,10 +7510,10 @@
         <v>21</v>
       </c>
       <c r="H252" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
       <c r="I252" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="253" spans="1:9">
@@ -7457,10 +7550,10 @@
         <v>106</v>
       </c>
       <c r="H254" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="I254" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="255" spans="1:9">
@@ -7480,13 +7573,13 @@
         <v>22</v>
       </c>
       <c r="F255" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="H255" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
       <c r="I255" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="256" spans="1:9">
@@ -7506,10 +7599,10 @@
         <v>107</v>
       </c>
       <c r="H256" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="I256" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="257" spans="1:9">
@@ -7529,13 +7622,13 @@
         <v>22</v>
       </c>
       <c r="F257" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="H257" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="I257" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="258" spans="1:9">
@@ -7555,13 +7648,13 @@
         <v>22</v>
       </c>
       <c r="F258" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="H258" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="I258" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="259" spans="1:9">
@@ -7581,10 +7674,10 @@
         <v>108</v>
       </c>
       <c r="H259" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="I259" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="260" spans="1:9">
@@ -7604,7 +7697,7 @@
         <v>26</v>
       </c>
       <c r="F260" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="261" spans="1:9">
@@ -7624,13 +7717,13 @@
         <v>22</v>
       </c>
       <c r="F261" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="H261" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
       <c r="I261" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="262" spans="1:9">
@@ -7650,13 +7743,13 @@
         <v>22</v>
       </c>
       <c r="F262" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H262" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="I262" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="263" spans="1:9">
@@ -7676,10 +7769,10 @@
         <v>109</v>
       </c>
       <c r="H263" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="I263" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="264" spans="1:9">
@@ -7699,10 +7792,10 @@
         <v>31</v>
       </c>
       <c r="H264" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="I264" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="265" spans="1:9">
@@ -7722,10 +7815,10 @@
         <v>31</v>
       </c>
       <c r="H265" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="I265" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="266" spans="1:9">
@@ -7745,10 +7838,10 @@
         <v>31</v>
       </c>
       <c r="H266" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="I266" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="267" spans="1:9">
@@ -7768,13 +7861,13 @@
         <v>88</v>
       </c>
       <c r="F267" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="H267" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="I267" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="268" spans="1:9">
@@ -7794,10 +7887,10 @@
         <v>31</v>
       </c>
       <c r="H268" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="I268" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="269" spans="1:9">
@@ -7817,10 +7910,10 @@
         <v>31</v>
       </c>
       <c r="H269" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="I269" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="270" spans="1:9">
@@ -7840,10 +7933,10 @@
         <v>31</v>
       </c>
       <c r="H270" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="I270" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="271" spans="1:9">
@@ -7863,10 +7956,10 @@
         <v>31</v>
       </c>
       <c r="H271" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="I271" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="272" spans="1:9">
@@ -7886,13 +7979,13 @@
         <v>22</v>
       </c>
       <c r="F272" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="H272" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="I272" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="273" spans="1:9">
@@ -7912,13 +8005,13 @@
         <v>22</v>
       </c>
       <c r="F273" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="H273" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="I273" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="274" spans="1:9">
@@ -7958,13 +8051,13 @@
         <v>41</v>
       </c>
       <c r="F275" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H275" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="I275" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="276" spans="1:9">
@@ -7984,13 +8077,13 @@
         <v>22</v>
       </c>
       <c r="F276" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H276" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="I276" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="277" spans="1:9">
@@ -8010,10 +8103,10 @@
         <v>31</v>
       </c>
       <c r="H277" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="I277" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="278" spans="1:9">
@@ -8033,10 +8126,10 @@
         <v>31</v>
       </c>
       <c r="H278" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="I278" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="279" spans="1:9">
@@ -8056,10 +8149,10 @@
         <v>58</v>
       </c>
       <c r="H279" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="I279" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="280" spans="1:9">
@@ -8079,13 +8172,13 @@
         <v>22</v>
       </c>
       <c r="F280" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="H280" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
       <c r="I280" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="281" spans="1:9">
@@ -8105,13 +8198,13 @@
         <v>22</v>
       </c>
       <c r="F281" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="H281" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="I281" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="282" spans="1:9">
@@ -8131,10 +8224,10 @@
         <v>31</v>
       </c>
       <c r="H282" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="I282" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="283" spans="1:9">
@@ -8154,13 +8247,13 @@
         <v>22</v>
       </c>
       <c r="F283" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="H283" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="I283" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="284" spans="1:9">
@@ -8180,10 +8273,10 @@
         <v>31</v>
       </c>
       <c r="H284" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="I284" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="285" spans="1:9">
@@ -8203,10 +8296,10 @@
         <v>31</v>
       </c>
       <c r="H285" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="I285" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="286" spans="1:9">
@@ -8226,10 +8319,10 @@
         <v>31</v>
       </c>
       <c r="H286" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="I286" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="287" spans="1:9">
@@ -8249,10 +8342,10 @@
         <v>31</v>
       </c>
       <c r="H287" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="I287" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="288" spans="1:9">
@@ -8272,10 +8365,10 @@
         <v>110</v>
       </c>
       <c r="H288" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="I288" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="289" spans="1:9">
@@ -8312,10 +8405,10 @@
         <v>27</v>
       </c>
       <c r="H290" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
       <c r="I290" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="291" spans="1:9">
@@ -8335,13 +8428,13 @@
         <v>22</v>
       </c>
       <c r="F291" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="H291" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="I291" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="292" spans="1:9">
@@ -8361,13 +8454,13 @@
         <v>26</v>
       </c>
       <c r="F292" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="H292" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
       <c r="I292" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="293" spans="1:9">
@@ -8387,10 +8480,10 @@
         <v>112</v>
       </c>
       <c r="H293" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="I293" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="294" spans="1:9">
@@ -8410,13 +8503,13 @@
         <v>22</v>
       </c>
       <c r="F294" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="H294" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
       <c r="I294" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="295" spans="1:9">
@@ -8436,7 +8529,7 @@
         <v>41</v>
       </c>
       <c r="F295" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="296" spans="1:9">
@@ -8456,7 +8549,7 @@
         <v>33</v>
       </c>
       <c r="F296" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="297" spans="1:9">
@@ -8476,13 +8569,13 @@
         <v>41</v>
       </c>
       <c r="F297" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="H297" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="I297" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="298" spans="1:9">
@@ -8519,10 +8612,10 @@
         <v>22</v>
       </c>
       <c r="H299" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
       <c r="I299" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="300" spans="1:9">
@@ -8542,13 +8635,13 @@
         <v>22</v>
       </c>
       <c r="F300" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H300" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
       <c r="I300" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="301" spans="1:9">
@@ -8568,13 +8661,13 @@
         <v>22</v>
       </c>
       <c r="F301" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="H301" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
       <c r="I301" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
     </row>
     <row r="302" spans="1:9">
@@ -8594,10 +8687,10 @@
         <v>114</v>
       </c>
       <c r="H302" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="I302" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="303" spans="1:9">
@@ -8617,10 +8710,10 @@
         <v>115</v>
       </c>
       <c r="H303" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="I303" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="304" spans="1:9">
@@ -8640,10 +8733,10 @@
         <v>54</v>
       </c>
       <c r="H304" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="I304" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="305" spans="1:9">
@@ -8663,10 +8756,10 @@
         <v>116</v>
       </c>
       <c r="H305" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="I305" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
     </row>
     <row r="306" spans="1:9">
@@ -8686,10 +8779,540 @@
         <v>117</v>
       </c>
       <c r="H306" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="I306" t="s">
-        <v>419</v>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="307" spans="1:9">
+      <c r="A307" s="1">
+        <v>305</v>
+      </c>
+      <c r="B307" s="2">
+        <v>42775</v>
+      </c>
+      <c r="C307" t="s">
+        <v>9</v>
+      </c>
+      <c r="D307" t="s">
+        <v>17</v>
+      </c>
+      <c r="E307" t="s">
+        <v>22</v>
+      </c>
+      <c r="F307" t="s">
+        <v>145</v>
+      </c>
+      <c r="H307" t="s">
+        <v>428</v>
+      </c>
+      <c r="I307" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="308" spans="1:9">
+      <c r="A308" s="1">
+        <v>306</v>
+      </c>
+      <c r="B308" s="2">
+        <v>42776</v>
+      </c>
+      <c r="C308" t="s">
+        <v>9</v>
+      </c>
+      <c r="D308" t="s">
+        <v>18</v>
+      </c>
+      <c r="E308" t="s">
+        <v>118</v>
+      </c>
+      <c r="H308" t="s">
+        <v>429</v>
+      </c>
+      <c r="I308" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="309" spans="1:9">
+      <c r="A309" s="1">
+        <v>307</v>
+      </c>
+      <c r="B309" s="2">
+        <v>42777</v>
+      </c>
+      <c r="C309" t="s">
+        <v>9</v>
+      </c>
+      <c r="D309" t="s">
+        <v>17</v>
+      </c>
+      <c r="E309" t="s">
+        <v>22</v>
+      </c>
+      <c r="F309" t="s">
+        <v>191</v>
+      </c>
+      <c r="H309" t="s">
+        <v>430</v>
+      </c>
+      <c r="I309" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="310" spans="1:9">
+      <c r="A310" s="1">
+        <v>308</v>
+      </c>
+      <c r="B310" s="2">
+        <v>42775</v>
+      </c>
+      <c r="C310" t="s">
+        <v>9</v>
+      </c>
+      <c r="D310" t="s">
+        <v>17</v>
+      </c>
+      <c r="E310" t="s">
+        <v>119</v>
+      </c>
+      <c r="H310" t="s">
+        <v>431</v>
+      </c>
+      <c r="I310" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="311" spans="1:9">
+      <c r="A311" s="1">
+        <v>309</v>
+      </c>
+      <c r="B311" s="2">
+        <v>42777</v>
+      </c>
+      <c r="C311" t="s">
+        <v>9</v>
+      </c>
+      <c r="D311" t="s">
+        <v>17</v>
+      </c>
+      <c r="E311" t="s">
+        <v>55</v>
+      </c>
+      <c r="H311" t="s">
+        <v>432</v>
+      </c>
+      <c r="I311" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="312" spans="1:9">
+      <c r="A312" s="1">
+        <v>310</v>
+      </c>
+      <c r="B312" s="2">
+        <v>42779</v>
+      </c>
+      <c r="C312" t="s">
+        <v>9</v>
+      </c>
+      <c r="D312" t="s">
+        <v>17</v>
+      </c>
+      <c r="E312" t="s">
+        <v>31</v>
+      </c>
+      <c r="H312" t="s">
+        <v>433</v>
+      </c>
+      <c r="I312" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="313" spans="1:9">
+      <c r="A313" s="1">
+        <v>311</v>
+      </c>
+      <c r="B313" s="2">
+        <v>42779</v>
+      </c>
+      <c r="C313" t="s">
+        <v>9</v>
+      </c>
+      <c r="D313" t="s">
+        <v>17</v>
+      </c>
+      <c r="E313" t="s">
+        <v>55</v>
+      </c>
+      <c r="H313" t="s">
+        <v>434</v>
+      </c>
+      <c r="I313" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="314" spans="1:9">
+      <c r="A314" s="1">
+        <v>312</v>
+      </c>
+      <c r="B314" s="2">
+        <v>42778</v>
+      </c>
+      <c r="C314" t="s">
+        <v>9</v>
+      </c>
+      <c r="D314" t="s">
+        <v>17</v>
+      </c>
+      <c r="E314" t="s">
+        <v>22</v>
+      </c>
+      <c r="F314" t="s">
+        <v>145</v>
+      </c>
+      <c r="H314" t="s">
+        <v>435</v>
+      </c>
+      <c r="I314" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="315" spans="1:9">
+      <c r="A315" s="1">
+        <v>313</v>
+      </c>
+      <c r="B315" s="2">
+        <v>42778</v>
+      </c>
+      <c r="C315" t="s">
+        <v>9</v>
+      </c>
+      <c r="D315" t="s">
+        <v>17</v>
+      </c>
+      <c r="E315" t="s">
+        <v>120</v>
+      </c>
+      <c r="H315" t="s">
+        <v>436</v>
+      </c>
+      <c r="I315" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="316" spans="1:9">
+      <c r="A316" s="1">
+        <v>314</v>
+      </c>
+      <c r="B316" s="2">
+        <v>42778</v>
+      </c>
+      <c r="C316" t="s">
+        <v>9</v>
+      </c>
+      <c r="D316" t="s">
+        <v>17</v>
+      </c>
+      <c r="E316" t="s">
+        <v>26</v>
+      </c>
+      <c r="F316" t="s">
+        <v>198</v>
+      </c>
+      <c r="H316" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="317" spans="1:9">
+      <c r="A317" s="1">
+        <v>315</v>
+      </c>
+      <c r="B317" s="2">
+        <v>42781</v>
+      </c>
+      <c r="C317" t="s">
+        <v>9</v>
+      </c>
+      <c r="D317" t="s">
+        <v>18</v>
+      </c>
+      <c r="E317" t="s">
+        <v>121</v>
+      </c>
+      <c r="H317" t="s">
+        <v>438</v>
+      </c>
+      <c r="I317" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="318" spans="1:9">
+      <c r="A318" s="1">
+        <v>316</v>
+      </c>
+      <c r="B318" s="2">
+        <v>42781</v>
+      </c>
+      <c r="C318" t="s">
+        <v>9</v>
+      </c>
+      <c r="D318" t="s">
+        <v>16</v>
+      </c>
+      <c r="E318" t="s">
+        <v>58</v>
+      </c>
+      <c r="H318" t="s">
+        <v>439</v>
+      </c>
+      <c r="I318" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="319" spans="1:9">
+      <c r="A319" s="1">
+        <v>317</v>
+      </c>
+      <c r="B319" s="2">
+        <v>42781</v>
+      </c>
+      <c r="C319" t="s">
+        <v>9</v>
+      </c>
+      <c r="D319" t="s">
+        <v>17</v>
+      </c>
+      <c r="E319" t="s">
+        <v>55</v>
+      </c>
+      <c r="H319" t="s">
+        <v>440</v>
+      </c>
+      <c r="I319" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="320" spans="1:9">
+      <c r="A320" s="1">
+        <v>318</v>
+      </c>
+      <c r="B320" s="2">
+        <v>42782</v>
+      </c>
+      <c r="C320" t="s">
+        <v>9</v>
+      </c>
+      <c r="D320" t="s">
+        <v>18</v>
+      </c>
+      <c r="E320" t="s">
+        <v>122</v>
+      </c>
+      <c r="H320" t="s">
+        <v>441</v>
+      </c>
+      <c r="I320" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="321" spans="1:9">
+      <c r="A321" s="1">
+        <v>319</v>
+      </c>
+      <c r="B321" s="2">
+        <v>42782</v>
+      </c>
+      <c r="C321" t="s">
+        <v>9</v>
+      </c>
+      <c r="D321" t="s">
+        <v>17</v>
+      </c>
+      <c r="E321" t="s">
+        <v>22</v>
+      </c>
+      <c r="F321" t="s">
+        <v>199</v>
+      </c>
+      <c r="H321" t="s">
+        <v>442</v>
+      </c>
+      <c r="I321" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="322" spans="1:9">
+      <c r="A322" s="1">
+        <v>320</v>
+      </c>
+      <c r="B322" s="2">
+        <v>42783</v>
+      </c>
+      <c r="C322" t="s">
+        <v>9</v>
+      </c>
+      <c r="D322" t="s">
+        <v>17</v>
+      </c>
+      <c r="E322" t="s">
+        <v>22</v>
+      </c>
+      <c r="F322" t="s">
+        <v>145</v>
+      </c>
+      <c r="H322" t="s">
+        <v>443</v>
+      </c>
+      <c r="I322" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="323" spans="1:9">
+      <c r="A323" s="1">
+        <v>321</v>
+      </c>
+      <c r="B323" s="2">
+        <v>42787</v>
+      </c>
+      <c r="C323" t="s">
+        <v>9</v>
+      </c>
+      <c r="D323" t="s">
+        <v>17</v>
+      </c>
+      <c r="E323" t="s">
+        <v>28</v>
+      </c>
+      <c r="F323" t="s">
+        <v>200</v>
+      </c>
+      <c r="H323" t="s">
+        <v>444</v>
+      </c>
+      <c r="I323" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="324" spans="1:9">
+      <c r="A324" s="1">
+        <v>322</v>
+      </c>
+      <c r="B324" s="2">
+        <v>42788</v>
+      </c>
+      <c r="C324" t="s">
+        <v>9</v>
+      </c>
+      <c r="D324" t="s">
+        <v>16</v>
+      </c>
+      <c r="E324" t="s">
+        <v>123</v>
+      </c>
+      <c r="H324" t="s">
+        <v>445</v>
+      </c>
+      <c r="I324" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="325" spans="1:9">
+      <c r="A325" s="1">
+        <v>323</v>
+      </c>
+      <c r="B325" s="2">
+        <v>42789</v>
+      </c>
+      <c r="C325" t="s">
+        <v>9</v>
+      </c>
+      <c r="D325" t="s">
+        <v>17</v>
+      </c>
+      <c r="E325" t="s">
+        <v>55</v>
+      </c>
+      <c r="H325" t="s">
+        <v>446</v>
+      </c>
+      <c r="I325" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="326" spans="1:9">
+      <c r="A326" s="1">
+        <v>324</v>
+      </c>
+      <c r="B326" s="2">
+        <v>42789</v>
+      </c>
+      <c r="C326" t="s">
+        <v>9</v>
+      </c>
+      <c r="D326" t="s">
+        <v>17</v>
+      </c>
+      <c r="E326" t="s">
+        <v>22</v>
+      </c>
+      <c r="F326" t="s">
+        <v>183</v>
+      </c>
+      <c r="H326" t="s">
+        <v>447</v>
+      </c>
+      <c r="I326" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="327" spans="1:9">
+      <c r="A327" s="1">
+        <v>325</v>
+      </c>
+      <c r="B327" s="2">
+        <v>42791</v>
+      </c>
+      <c r="C327" t="s">
+        <v>9</v>
+      </c>
+      <c r="D327" t="s">
+        <v>17</v>
+      </c>
+      <c r="E327" t="s">
+        <v>22</v>
+      </c>
+      <c r="F327" t="s">
+        <v>145</v>
+      </c>
+      <c r="H327" t="s">
+        <v>448</v>
+      </c>
+      <c r="I327" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="328" spans="1:9">
+      <c r="A328" s="1">
+        <v>326</v>
+      </c>
+      <c r="B328" s="2">
+        <v>42793</v>
+      </c>
+      <c r="C328" t="s">
+        <v>9</v>
+      </c>
+      <c r="D328" t="s">
+        <v>17</v>
+      </c>
+      <c r="E328" t="s">
+        <v>54</v>
+      </c>
+      <c r="H328" t="s">
+        <v>449</v>
+      </c>
+      <c r="I328" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
budget charts now pull data from budget tracking google sheet
</commit_message>
<xml_diff>
--- a/xlsx/OTP_feedback_tracking_cleaned_no_pi.xlsx
+++ b/xlsx/OTP_feedback_tracking_cleaned_no_pi.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="466">
   <si>
     <t>Date Received</t>
   </si>
@@ -388,6 +388,15 @@
     <t>Would like "Turn left" and "Turn rigth" directions</t>
   </si>
   <si>
+    <t>"EXCELLENT!!!"</t>
+  </si>
+  <si>
+    <t>Wanted to know why MAX platforms have 2 stop IDs</t>
+  </si>
+  <si>
+    <t>"Thanks again"</t>
+  </si>
+  <si>
     <t>Location outside district</t>
   </si>
   <si>
@@ -619,6 +628,9 @@
     <t>User and GIS team can't replicate</t>
   </si>
   <si>
+    <t>Routed on footway that is too rough to use</t>
+  </si>
+  <si>
     <t>Vancouver</t>
   </si>
   <si>
@@ -1364,6 +1376,33 @@
   </si>
   <si>
     <t>https://trimet.org/#planner/results/from=6600+N+BOSTON+AVE%2C+Portland%3A%3A45.570885%2C-122.69117&amp;to=Pioneer+Square+South+MAX+Station+E%2C+Portland+(Stop+ID+8334)%3A%3A45.518497%2C-122.679146&amp;m=am&amp;walk=1260&amp;arr=A</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#planner/results/from=775+NE+5TH+ST%2C+GRESHAM+97030%3A%3A45.501008%2C-122.423025&amp;to=Hollywood%2FNE+42nd+Ave+Transit+Center%2C+Portland%3A%3A45.53328%2C-122.620636&amp;mode=RAIL%2CTRAM%2CSUBWAY%2CFUNICULAR%2CGONDOLA%2CWALK&amp;m=pm&amp;walk=1260&amp;arr=A</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=SW+Lombard+%26+Allen+-+Stop+ID+3455%3A%3A45.47699%2C-122.800202&amp;to=7881+SW+CAPITOL+HWY%3A%3A45.467623%2C-122.714682&amp;m=am&amp;walk=1260&amp;arr=D</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#/planner/results/itin_num=2&amp;from=19725%20RIVER%20RD,%20Gladstone::45.376446,-122.60503&amp;to=SE%20122nd%20%26%20Powell%20N,%20Portland%20(Stop%20ID%206655)::45.497345,-122.537506&amp;Walk=1260&amp;Arr=A</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#planner/results/from=1500+SW+5TH+AVE%2C+PORTLAND%3A%3A45.513468%2C-122.680474&amp;to=8470+SW+OLESON+RD%2C+Portland&amp;m=am&amp;walk=1260&amp;arr=A</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#planner/results/from=SW+Bull+Mountain+Rd+%26+Oregon+Route+99W%2C+Tigard%3A%3A45.414692%2C-122.791534&amp;to=Vancouver%2C+WA&amp;m=am&amp;walk=840&amp;arr=D</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=Clackamas+Town+Ctr+%26+Clackamas+Town+Center+TC%2C+Clackamas+County%3A%3A45.43555%2C-122.56904&amp;to=NE+7th+Ave+MAX+Station+W%2C+Portland+(Stop+ID+8375)%3A%3A45.53015%2C-122.65828&amp;mode=RAIL%2CTRAM%2CSUBWAY%2CFUNICULAR%2CGONDOLA%2CWALK&amp;m=am&amp;walk=1260&amp;arr=A</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#planner/results/from=8885+SW+CANYON+RD%2C+Portland%3A%3A45.49791%2C-122.768684&amp;to=1511+SW+PARK+AVE%2C+Portland%3A%3A45.514206%2C-122.68472&amp;m=pm&amp;walk=1260&amp;arr=A</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#/planner/results/itin_num=2&amp;from=3030</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=3508+NE+BROADWAY%2C+Portland%3A%3A45.53481%2C-122.628&amp;to=3911+SE+MILWAUKIE+AVE%2C+Portland%3A%3A45.494194%2C-122.65303</t>
   </si>
   <si>
     <t>Weekday</t>
@@ -1734,7 +1773,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I328"/>
+  <dimension ref="A1:I337"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1830,13 +1869,13 @@
         <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G4" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H4" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1856,13 +1895,13 @@
         <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G5" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="H5" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1882,10 +1921,10 @@
         <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="I6" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1945,7 +1984,7 @@
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1965,13 +2004,13 @@
         <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G10" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H10" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2008,13 +2047,13 @@
         <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G12" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H12" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2034,7 +2073,7 @@
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2054,7 +2093,7 @@
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2094,13 +2133,13 @@
         <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G16" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H16" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2137,7 +2176,7 @@
         <v>22</v>
       </c>
       <c r="F18" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2157,10 +2196,10 @@
         <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H19" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2180,13 +2219,13 @@
         <v>23</v>
       </c>
       <c r="F20" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G20" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H20" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2206,10 +2245,10 @@
         <v>26</v>
       </c>
       <c r="F21" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H21" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2229,13 +2268,13 @@
         <v>23</v>
       </c>
       <c r="F22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G22" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H22" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2255,13 +2294,13 @@
         <v>23</v>
       </c>
       <c r="F23" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G23" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="H23" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2281,7 +2320,7 @@
         <v>22</v>
       </c>
       <c r="F24" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2318,7 +2357,7 @@
         <v>33</v>
       </c>
       <c r="F26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2338,10 +2377,10 @@
         <v>26</v>
       </c>
       <c r="F27" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H27" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2361,10 +2400,10 @@
         <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="H28" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2384,13 +2423,13 @@
         <v>23</v>
       </c>
       <c r="F29" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G29" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H29" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2410,13 +2449,13 @@
         <v>23</v>
       </c>
       <c r="F30" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G30" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H30" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2453,13 +2492,13 @@
         <v>23</v>
       </c>
       <c r="F32" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G32" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="H32" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2479,10 +2518,10 @@
         <v>26</v>
       </c>
       <c r="F33" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="H33" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2519,10 +2558,10 @@
         <v>23</v>
       </c>
       <c r="F35" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G35" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2542,10 +2581,10 @@
         <v>23</v>
       </c>
       <c r="F36" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G36" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2565,10 +2604,10 @@
         <v>26</v>
       </c>
       <c r="F37" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H37" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2622,10 +2661,10 @@
         <v>26</v>
       </c>
       <c r="F40" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="H40" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2645,13 +2684,13 @@
         <v>23</v>
       </c>
       <c r="F41" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G41" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="H41" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2671,13 +2710,13 @@
         <v>23</v>
       </c>
       <c r="F42" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G42" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="H42" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2697,7 +2736,7 @@
         <v>37</v>
       </c>
       <c r="F43" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2717,10 +2756,10 @@
         <v>26</v>
       </c>
       <c r="F44" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="H44" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2740,10 +2779,10 @@
         <v>26</v>
       </c>
       <c r="F45" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="H45" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2763,7 +2802,7 @@
         <v>22</v>
       </c>
       <c r="F46" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2783,10 +2822,10 @@
         <v>26</v>
       </c>
       <c r="F47" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H47" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2823,10 +2862,10 @@
         <v>26</v>
       </c>
       <c r="F49" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="H49" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2846,7 +2885,7 @@
         <v>22</v>
       </c>
       <c r="F50" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2923,13 +2962,13 @@
         <v>23</v>
       </c>
       <c r="F54" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G54" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H54" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2949,10 +2988,10 @@
         <v>26</v>
       </c>
       <c r="F55" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H55" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -3026,7 +3065,7 @@
         <v>41</v>
       </c>
       <c r="F59" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -3046,7 +3085,7 @@
         <v>41</v>
       </c>
       <c r="F60" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -3103,13 +3142,13 @@
         <v>23</v>
       </c>
       <c r="F63" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G63" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H63" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -3129,10 +3168,10 @@
         <v>44</v>
       </c>
       <c r="H64" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="I64" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -3152,10 +3191,10 @@
         <v>45</v>
       </c>
       <c r="H65" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="I65" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -3192,7 +3231,7 @@
         <v>26</v>
       </c>
       <c r="F67" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -3212,13 +3251,13 @@
         <v>46</v>
       </c>
       <c r="F68" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H68" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="I68" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -3238,13 +3277,13 @@
         <v>22</v>
       </c>
       <c r="F69" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H69" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="I69" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -3284,10 +3323,10 @@
         <v>44</v>
       </c>
       <c r="H71" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="I71" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -3307,13 +3346,13 @@
         <v>47</v>
       </c>
       <c r="F72" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H72" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="I72" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -3333,13 +3372,13 @@
         <v>47</v>
       </c>
       <c r="F73" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="H73" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="I73" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -3359,7 +3398,7 @@
         <v>22</v>
       </c>
       <c r="F74" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -3379,10 +3418,10 @@
         <v>48</v>
       </c>
       <c r="H75" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="I75" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -3402,10 +3441,10 @@
         <v>49</v>
       </c>
       <c r="H76" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="I76" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -3425,10 +3464,10 @@
         <v>50</v>
       </c>
       <c r="H77" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="I77" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -3465,10 +3504,10 @@
         <v>52</v>
       </c>
       <c r="H79" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="I79" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -3488,10 +3527,10 @@
         <v>21</v>
       </c>
       <c r="H80" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="I80" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -3514,10 +3553,10 @@
         <v>20</v>
       </c>
       <c r="H81" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="I81" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -3537,10 +3576,10 @@
         <v>53</v>
       </c>
       <c r="H82" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="I82" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3560,10 +3599,10 @@
         <v>54</v>
       </c>
       <c r="H83" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="I83" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -3583,10 +3622,10 @@
         <v>31</v>
       </c>
       <c r="H84" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="I84" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -3606,10 +3645,10 @@
         <v>55</v>
       </c>
       <c r="H85" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="I85" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -3629,10 +3668,10 @@
         <v>56</v>
       </c>
       <c r="H86" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="I86" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -3655,10 +3694,10 @@
         <v>20</v>
       </c>
       <c r="H87" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="I87" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -3678,13 +3717,13 @@
         <v>22</v>
       </c>
       <c r="F88" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H88" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="I88" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -3707,10 +3746,10 @@
         <v>20</v>
       </c>
       <c r="H89" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="I89" t="s">
-        <v>452</v>
+        <v>465</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -3730,10 +3769,10 @@
         <v>58</v>
       </c>
       <c r="H90" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="I90" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3753,7 +3792,7 @@
         <v>22</v>
       </c>
       <c r="F91" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -3813,10 +3852,10 @@
         <v>20</v>
       </c>
       <c r="H94" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="I94" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -3836,13 +3875,13 @@
         <v>22</v>
       </c>
       <c r="F95" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="H95" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="I95" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -3862,13 +3901,13 @@
         <v>22</v>
       </c>
       <c r="F96" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H96" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="I96" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -3888,13 +3927,13 @@
         <v>60</v>
       </c>
       <c r="F97" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="H97" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="I97" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -3914,10 +3953,10 @@
         <v>61</v>
       </c>
       <c r="H98" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="I98" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -3937,13 +3976,13 @@
         <v>22</v>
       </c>
       <c r="F99" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H99" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="I99" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -3963,10 +4002,10 @@
         <v>54</v>
       </c>
       <c r="H100" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="I100" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -3986,7 +4025,7 @@
         <v>28</v>
       </c>
       <c r="F101" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -4006,10 +4045,10 @@
         <v>54</v>
       </c>
       <c r="H102" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="I102" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -4029,13 +4068,13 @@
         <v>62</v>
       </c>
       <c r="F103" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H103" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="I103" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -4055,13 +4094,13 @@
         <v>62</v>
       </c>
       <c r="F104" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H104" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="I104" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -4081,10 +4120,10 @@
         <v>35</v>
       </c>
       <c r="H105" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="I105" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -4104,13 +4143,13 @@
         <v>62</v>
       </c>
       <c r="F106" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H106" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="I106" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -4130,13 +4169,13 @@
         <v>41</v>
       </c>
       <c r="F107" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H107" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="I107" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -4156,13 +4195,13 @@
         <v>22</v>
       </c>
       <c r="F108" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H108" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="I108" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -4182,13 +4221,13 @@
         <v>22</v>
       </c>
       <c r="F109" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H109" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="I109" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -4208,10 +4247,10 @@
         <v>31</v>
       </c>
       <c r="H110" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="I110" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -4231,10 +4270,10 @@
         <v>23</v>
       </c>
       <c r="H111" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="I111" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -4254,7 +4293,7 @@
         <v>26</v>
       </c>
       <c r="F112" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="113" spans="1:9">
@@ -4274,10 +4313,10 @@
         <v>44</v>
       </c>
       <c r="H113" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="I113" t="s">
-        <v>452</v>
+        <v>465</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -4314,13 +4353,13 @@
         <v>64</v>
       </c>
       <c r="F115" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H115" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="I115" t="s">
-        <v>452</v>
+        <v>465</v>
       </c>
     </row>
     <row r="116" spans="1:9">
@@ -4357,7 +4396,7 @@
         <v>66</v>
       </c>
       <c r="H117" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="118" spans="1:9">
@@ -4377,10 +4416,10 @@
         <v>45</v>
       </c>
       <c r="H118" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="I118" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="119" spans="1:9">
@@ -4417,10 +4456,10 @@
         <v>67</v>
       </c>
       <c r="H120" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="I120" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="121" spans="1:9">
@@ -4440,7 +4479,7 @@
         <v>22</v>
       </c>
       <c r="F121" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="122" spans="1:9">
@@ -4480,10 +4519,10 @@
         <v>20</v>
       </c>
       <c r="H123" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="I123" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="124" spans="1:9">
@@ -4503,10 +4542,10 @@
         <v>69</v>
       </c>
       <c r="H124" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="I124" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="125" spans="1:9">
@@ -4526,13 +4565,13 @@
         <v>26</v>
       </c>
       <c r="F125" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="H125" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="I125" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="126" spans="1:9">
@@ -4552,10 +4591,10 @@
         <v>35</v>
       </c>
       <c r="H126" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="I126" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="127" spans="1:9">
@@ -4592,10 +4631,10 @@
         <v>27</v>
       </c>
       <c r="H128" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="I128" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="129" spans="1:9">
@@ -4615,13 +4654,13 @@
         <v>22</v>
       </c>
       <c r="F129" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H129" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="I129" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -4641,10 +4680,10 @@
         <v>70</v>
       </c>
       <c r="H130" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="I130" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="131" spans="1:9">
@@ -4664,10 +4703,10 @@
         <v>71</v>
       </c>
       <c r="H131" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="I131" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="132" spans="1:9">
@@ -4687,13 +4726,13 @@
         <v>22</v>
       </c>
       <c r="F132" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H132" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="I132" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="133" spans="1:9">
@@ -4713,10 +4752,10 @@
         <v>26</v>
       </c>
       <c r="F133" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H133" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="134" spans="1:9">
@@ -4736,7 +4775,7 @@
         <v>33</v>
       </c>
       <c r="F134" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="135" spans="1:9">
@@ -4776,10 +4815,10 @@
         <v>54</v>
       </c>
       <c r="H136" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="I136" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="137" spans="1:9">
@@ -4799,13 +4838,13 @@
         <v>72</v>
       </c>
       <c r="F137" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="H137" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="I137" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="138" spans="1:9">
@@ -4825,10 +4864,10 @@
         <v>26</v>
       </c>
       <c r="F138" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="H138" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="139" spans="1:9">
@@ -4848,10 +4887,10 @@
         <v>26</v>
       </c>
       <c r="F139" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H139" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="140" spans="1:9">
@@ -4871,13 +4910,13 @@
         <v>73</v>
       </c>
       <c r="F140" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H140" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="I140" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="141" spans="1:9">
@@ -4897,13 +4936,13 @@
         <v>22</v>
       </c>
       <c r="F141" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H141" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="I141" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="142" spans="1:9">
@@ -4943,10 +4982,10 @@
         <v>68</v>
       </c>
       <c r="H143" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="I143" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -4966,10 +5005,10 @@
         <v>52</v>
       </c>
       <c r="H144" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="I144" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -4989,10 +5028,10 @@
         <v>21</v>
       </c>
       <c r="H145" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="I145" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -5012,13 +5051,13 @@
         <v>22</v>
       </c>
       <c r="F146" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H146" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="I146" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -5038,10 +5077,10 @@
         <v>26</v>
       </c>
       <c r="F147" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="H147" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -5061,10 +5100,10 @@
         <v>33</v>
       </c>
       <c r="F148" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="H148" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -5084,7 +5123,7 @@
         <v>33</v>
       </c>
       <c r="F149" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -5104,7 +5143,7 @@
         <v>22</v>
       </c>
       <c r="F150" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -5124,13 +5163,13 @@
         <v>22</v>
       </c>
       <c r="F151" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H151" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="I151" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -5150,13 +5189,13 @@
         <v>22</v>
       </c>
       <c r="F152" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H152" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="I152" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -5176,13 +5215,13 @@
         <v>41</v>
       </c>
       <c r="F153" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H153" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="I153" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="154" spans="1:9">
@@ -5202,7 +5241,7 @@
         <v>26</v>
       </c>
       <c r="F154" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -5222,13 +5261,13 @@
         <v>22</v>
       </c>
       <c r="F155" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H155" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="I155" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="156" spans="1:9">
@@ -5248,10 +5287,10 @@
         <v>74</v>
       </c>
       <c r="H156" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="I156" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="157" spans="1:9">
@@ -5271,10 +5310,10 @@
         <v>75</v>
       </c>
       <c r="H157" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="I157" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="158" spans="1:9">
@@ -5311,13 +5350,13 @@
         <v>76</v>
       </c>
       <c r="F159" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H159" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="I159" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="160" spans="1:9">
@@ -5337,10 +5376,10 @@
         <v>77</v>
       </c>
       <c r="H160" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="I160" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="161" spans="1:9">
@@ -5360,13 +5399,13 @@
         <v>22</v>
       </c>
       <c r="F161" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H161" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="I161" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="162" spans="1:9">
@@ -5386,10 +5425,10 @@
         <v>78</v>
       </c>
       <c r="H162" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="I162" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="163" spans="1:9">
@@ -5409,13 +5448,13 @@
         <v>22</v>
       </c>
       <c r="F163" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H163" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="I163" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="164" spans="1:9">
@@ -5455,7 +5494,7 @@
         <v>20</v>
       </c>
       <c r="H165" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="166" spans="1:9">
@@ -5475,13 +5514,13 @@
         <v>22</v>
       </c>
       <c r="F166" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H166" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="I166" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="167" spans="1:9">
@@ -5518,13 +5557,13 @@
         <v>23</v>
       </c>
       <c r="F168" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G168" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="H168" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="169" spans="1:9">
@@ -5544,13 +5583,13 @@
         <v>41</v>
       </c>
       <c r="F169" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="H169" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="I169" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="170" spans="1:9">
@@ -5570,10 +5609,10 @@
         <v>31</v>
       </c>
       <c r="H170" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="I170" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="171" spans="1:9">
@@ -5593,10 +5632,10 @@
         <v>45</v>
       </c>
       <c r="H171" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="I171" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="172" spans="1:9">
@@ -5616,10 +5655,10 @@
         <v>81</v>
       </c>
       <c r="H172" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="I172" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="173" spans="1:9">
@@ -5639,10 +5678,10 @@
         <v>58</v>
       </c>
       <c r="H173" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="I173" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="174" spans="1:9">
@@ -5662,13 +5701,13 @@
         <v>31</v>
       </c>
       <c r="F174" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H174" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="I174" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="175" spans="1:9">
@@ -5691,10 +5730,10 @@
         <v>20</v>
       </c>
       <c r="H175" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="I175" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="176" spans="1:9">
@@ -5714,13 +5753,13 @@
         <v>22</v>
       </c>
       <c r="F176" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H176" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="I176" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="177" spans="1:9">
@@ -5740,7 +5779,7 @@
         <v>26</v>
       </c>
       <c r="F177" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="178" spans="1:9">
@@ -5760,10 +5799,10 @@
         <v>82</v>
       </c>
       <c r="H178" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="I178" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="179" spans="1:9">
@@ -5783,10 +5822,10 @@
         <v>83</v>
       </c>
       <c r="H179" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="I179" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="180" spans="1:9">
@@ -5806,13 +5845,13 @@
         <v>41</v>
       </c>
       <c r="F180" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H180" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="I180" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="181" spans="1:9">
@@ -5832,13 +5871,13 @@
         <v>41</v>
       </c>
       <c r="F181" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H181" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="I181" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="182" spans="1:9">
@@ -5861,10 +5900,10 @@
         <v>20</v>
       </c>
       <c r="H182" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="I182" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="183" spans="1:9">
@@ -5884,10 +5923,10 @@
         <v>23</v>
       </c>
       <c r="F183" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G183" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="184" spans="1:9">
@@ -5907,10 +5946,10 @@
         <v>84</v>
       </c>
       <c r="H184" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="I184" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="185" spans="1:9">
@@ -5930,7 +5969,7 @@
         <v>22</v>
       </c>
       <c r="F185" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="186" spans="1:9">
@@ -5950,10 +5989,10 @@
         <v>85</v>
       </c>
       <c r="H186" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="I186" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="187" spans="1:9">
@@ -5973,13 +6012,13 @@
         <v>86</v>
       </c>
       <c r="F187" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H187" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="I187" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="188" spans="1:9">
@@ -5999,13 +6038,13 @@
         <v>22</v>
       </c>
       <c r="F188" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="H188" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="I188" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="189" spans="1:9">
@@ -6025,10 +6064,10 @@
         <v>87</v>
       </c>
       <c r="H189" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="I189" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="190" spans="1:9">
@@ -6048,10 +6087,10 @@
         <v>20</v>
       </c>
       <c r="H190" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="I190" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="191" spans="1:9">
@@ -6071,10 +6110,10 @@
         <v>88</v>
       </c>
       <c r="F191" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H191" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="192" spans="1:9">
@@ -6094,10 +6133,10 @@
         <v>45</v>
       </c>
       <c r="H192" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="I192" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="193" spans="1:9">
@@ -6117,10 +6156,10 @@
         <v>89</v>
       </c>
       <c r="H193" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="I193" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="194" spans="1:9">
@@ -6143,10 +6182,10 @@
         <v>20</v>
       </c>
       <c r="H194" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="I194" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="195" spans="1:9">
@@ -6166,10 +6205,10 @@
         <v>21</v>
       </c>
       <c r="H195" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="I195" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="196" spans="1:9">
@@ -6189,13 +6228,13 @@
         <v>41</v>
       </c>
       <c r="F196" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H196" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="I196" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="197" spans="1:9">
@@ -6215,13 +6254,13 @@
         <v>22</v>
       </c>
       <c r="F197" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H197" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="I197" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="198" spans="1:9">
@@ -6241,10 +6280,10 @@
         <v>54</v>
       </c>
       <c r="H198" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="I198" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="199" spans="1:9">
@@ -6264,13 +6303,13 @@
         <v>22</v>
       </c>
       <c r="F199" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H199" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="I199" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="200" spans="1:9">
@@ -6290,13 +6329,13 @@
         <v>22</v>
       </c>
       <c r="F200" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H200" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="I200" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="201" spans="1:9">
@@ -6316,13 +6355,13 @@
         <v>22</v>
       </c>
       <c r="F201" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H201" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="I201" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="202" spans="1:9">
@@ -6342,13 +6381,13 @@
         <v>90</v>
       </c>
       <c r="F202" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H202" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="I202" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="203" spans="1:9">
@@ -6368,10 +6407,10 @@
         <v>55</v>
       </c>
       <c r="H203" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="I203" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="204" spans="1:9">
@@ -6391,10 +6430,10 @@
         <v>55</v>
       </c>
       <c r="H204" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="I204" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="205" spans="1:9">
@@ -6414,10 +6453,10 @@
         <v>54</v>
       </c>
       <c r="H205" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="I205" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="206" spans="1:9">
@@ -6437,10 +6476,10 @@
         <v>54</v>
       </c>
       <c r="H206" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="I206" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="207" spans="1:9">
@@ -6460,10 +6499,10 @@
         <v>31</v>
       </c>
       <c r="H207" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="I207" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="208" spans="1:9">
@@ -6483,7 +6522,7 @@
         <v>91</v>
       </c>
       <c r="F208" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="209" spans="1:9">
@@ -6503,10 +6542,10 @@
         <v>92</v>
       </c>
       <c r="H209" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="I209" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="210" spans="1:9">
@@ -6526,10 +6565,10 @@
         <v>35</v>
       </c>
       <c r="H210" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="I210" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="211" spans="1:9">
@@ -6549,10 +6588,10 @@
         <v>54</v>
       </c>
       <c r="H211" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="I211" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="212" spans="1:9">
@@ -6572,13 +6611,13 @@
         <v>22</v>
       </c>
       <c r="F212" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H212" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="I212" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="213" spans="1:9">
@@ -6598,13 +6637,13 @@
         <v>22</v>
       </c>
       <c r="F213" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H213" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="I213" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="214" spans="1:9">
@@ -6624,10 +6663,10 @@
         <v>54</v>
       </c>
       <c r="H214" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="I214" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="215" spans="1:9">
@@ -6647,13 +6686,13 @@
         <v>22</v>
       </c>
       <c r="F215" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H215" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="I215" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="216" spans="1:9">
@@ -6673,10 +6712,10 @@
         <v>93</v>
       </c>
       <c r="H216" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="I216" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="217" spans="1:9">
@@ -6696,13 +6735,13 @@
         <v>94</v>
       </c>
       <c r="F217" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H217" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="I217" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="218" spans="1:9">
@@ -6722,13 +6761,13 @@
         <v>22</v>
       </c>
       <c r="F218" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H218" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="I218" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="219" spans="1:9">
@@ -6748,13 +6787,13 @@
         <v>95</v>
       </c>
       <c r="F219" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H219" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="I219" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="220" spans="1:9">
@@ -6774,10 +6813,10 @@
         <v>31</v>
       </c>
       <c r="H220" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="I220" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="221" spans="1:9">
@@ -6797,13 +6836,13 @@
         <v>95</v>
       </c>
       <c r="F221" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H221" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="I221" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="222" spans="1:9">
@@ -6823,13 +6862,13 @@
         <v>22</v>
       </c>
       <c r="F222" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H222" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="I222" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="223" spans="1:9">
@@ -6849,13 +6888,13 @@
         <v>22</v>
       </c>
       <c r="F223" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H223" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="I223" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="224" spans="1:9">
@@ -6892,13 +6931,13 @@
         <v>95</v>
       </c>
       <c r="F225" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H225" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="I225" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="226" spans="1:9">
@@ -6935,13 +6974,13 @@
         <v>95</v>
       </c>
       <c r="F227" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H227" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="I227" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="228" spans="1:9">
@@ -6978,10 +7017,10 @@
         <v>98</v>
       </c>
       <c r="H229" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="I229" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="230" spans="1:9">
@@ -7001,13 +7040,13 @@
         <v>95</v>
       </c>
       <c r="F230" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H230" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="I230" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="231" spans="1:9">
@@ -7027,10 +7066,10 @@
         <v>99</v>
       </c>
       <c r="H231" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="I231" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="232" spans="1:9">
@@ -7084,10 +7123,10 @@
         <v>101</v>
       </c>
       <c r="H234" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="I234" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="235" spans="1:9">
@@ -7107,13 +7146,13 @@
         <v>102</v>
       </c>
       <c r="F235" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H235" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="I235" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="236" spans="1:9">
@@ -7133,13 +7172,13 @@
         <v>22</v>
       </c>
       <c r="F236" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H236" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="I236" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="237" spans="1:9">
@@ -7159,10 +7198,10 @@
         <v>103</v>
       </c>
       <c r="H237" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="I237" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="238" spans="1:9">
@@ -7182,13 +7221,13 @@
         <v>22</v>
       </c>
       <c r="F238" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H238" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="I238" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="239" spans="1:9">
@@ -7208,13 +7247,13 @@
         <v>22</v>
       </c>
       <c r="F239" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H239" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="I239" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="240" spans="1:9">
@@ -7234,10 +7273,10 @@
         <v>104</v>
       </c>
       <c r="H240" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="I240" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="241" spans="1:9">
@@ -7257,10 +7296,10 @@
         <v>45</v>
       </c>
       <c r="H241" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="I241" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="242" spans="1:9">
@@ -7300,10 +7339,10 @@
         <v>58</v>
       </c>
       <c r="H243" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="I243" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="244" spans="1:9">
@@ -7323,7 +7362,7 @@
         <v>22</v>
       </c>
       <c r="F244" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="245" spans="1:9">
@@ -7343,13 +7382,13 @@
         <v>91</v>
       </c>
       <c r="F245" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="H245" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="I245" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="246" spans="1:9">
@@ -7369,13 +7408,13 @@
         <v>22</v>
       </c>
       <c r="F246" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="H246" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="I246" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="247" spans="1:9">
@@ -7395,10 +7434,10 @@
         <v>56</v>
       </c>
       <c r="H247" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="I247" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="248" spans="1:9">
@@ -7418,7 +7457,7 @@
         <v>41</v>
       </c>
       <c r="F248" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="249" spans="1:9">
@@ -7438,13 +7477,13 @@
         <v>22</v>
       </c>
       <c r="F249" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H249" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="I249" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="250" spans="1:9">
@@ -7484,13 +7523,13 @@
         <v>22</v>
       </c>
       <c r="F251" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="H251" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="I251" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="252" spans="1:9">
@@ -7510,10 +7549,10 @@
         <v>21</v>
       </c>
       <c r="H252" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="I252" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="253" spans="1:9">
@@ -7550,10 +7589,10 @@
         <v>106</v>
       </c>
       <c r="H254" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="I254" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="255" spans="1:9">
@@ -7573,13 +7612,13 @@
         <v>22</v>
       </c>
       <c r="F255" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="H255" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="I255" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="256" spans="1:9">
@@ -7599,10 +7638,10 @@
         <v>107</v>
       </c>
       <c r="H256" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="I256" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="257" spans="1:9">
@@ -7622,13 +7661,13 @@
         <v>22</v>
       </c>
       <c r="F257" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="H257" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="I257" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="258" spans="1:9">
@@ -7648,13 +7687,13 @@
         <v>22</v>
       </c>
       <c r="F258" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="H258" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="I258" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="259" spans="1:9">
@@ -7674,10 +7713,10 @@
         <v>108</v>
       </c>
       <c r="H259" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="I259" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="260" spans="1:9">
@@ -7697,7 +7736,7 @@
         <v>26</v>
       </c>
       <c r="F260" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="261" spans="1:9">
@@ -7717,13 +7756,13 @@
         <v>22</v>
       </c>
       <c r="F261" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="H261" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="I261" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="262" spans="1:9">
@@ -7743,13 +7782,13 @@
         <v>22</v>
       </c>
       <c r="F262" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H262" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="I262" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="263" spans="1:9">
@@ -7769,10 +7808,10 @@
         <v>109</v>
       </c>
       <c r="H263" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="I263" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="264" spans="1:9">
@@ -7792,10 +7831,10 @@
         <v>31</v>
       </c>
       <c r="H264" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="I264" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="265" spans="1:9">
@@ -7815,10 +7854,10 @@
         <v>31</v>
       </c>
       <c r="H265" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="I265" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="266" spans="1:9">
@@ -7838,10 +7877,10 @@
         <v>31</v>
       </c>
       <c r="H266" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="I266" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="267" spans="1:9">
@@ -7861,13 +7900,13 @@
         <v>88</v>
       </c>
       <c r="F267" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="H267" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="I267" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="268" spans="1:9">
@@ -7887,10 +7926,10 @@
         <v>31</v>
       </c>
       <c r="H268" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="I268" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="269" spans="1:9">
@@ -7910,10 +7949,10 @@
         <v>31</v>
       </c>
       <c r="H269" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="I269" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="270" spans="1:9">
@@ -7933,10 +7972,10 @@
         <v>31</v>
       </c>
       <c r="H270" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="I270" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="271" spans="1:9">
@@ -7956,10 +7995,10 @@
         <v>31</v>
       </c>
       <c r="H271" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="I271" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="272" spans="1:9">
@@ -7979,13 +8018,13 @@
         <v>22</v>
       </c>
       <c r="F272" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H272" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="I272" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="273" spans="1:9">
@@ -8005,13 +8044,13 @@
         <v>22</v>
       </c>
       <c r="F273" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H273" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="I273" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="274" spans="1:9">
@@ -8051,13 +8090,13 @@
         <v>41</v>
       </c>
       <c r="F275" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="H275" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="I275" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="276" spans="1:9">
@@ -8077,13 +8116,13 @@
         <v>22</v>
       </c>
       <c r="F276" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H276" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="I276" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="277" spans="1:9">
@@ -8103,10 +8142,10 @@
         <v>31</v>
       </c>
       <c r="H277" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="I277" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="278" spans="1:9">
@@ -8126,10 +8165,10 @@
         <v>31</v>
       </c>
       <c r="H278" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="I278" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="279" spans="1:9">
@@ -8149,10 +8188,10 @@
         <v>58</v>
       </c>
       <c r="H279" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="I279" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="280" spans="1:9">
@@ -8172,13 +8211,13 @@
         <v>22</v>
       </c>
       <c r="F280" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H280" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="I280" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="281" spans="1:9">
@@ -8198,13 +8237,13 @@
         <v>22</v>
       </c>
       <c r="F281" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H281" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="I281" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="282" spans="1:9">
@@ -8224,10 +8263,10 @@
         <v>31</v>
       </c>
       <c r="H282" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="I282" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="283" spans="1:9">
@@ -8247,13 +8286,13 @@
         <v>22</v>
       </c>
       <c r="F283" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="H283" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="I283" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="284" spans="1:9">
@@ -8273,10 +8312,10 @@
         <v>31</v>
       </c>
       <c r="H284" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="I284" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="285" spans="1:9">
@@ -8296,10 +8335,10 @@
         <v>31</v>
       </c>
       <c r="H285" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="I285" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="286" spans="1:9">
@@ -8319,10 +8358,10 @@
         <v>31</v>
       </c>
       <c r="H286" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="I286" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="287" spans="1:9">
@@ -8342,10 +8381,10 @@
         <v>31</v>
       </c>
       <c r="H287" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="I287" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="288" spans="1:9">
@@ -8365,10 +8404,10 @@
         <v>110</v>
       </c>
       <c r="H288" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="I288" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="289" spans="1:9">
@@ -8405,10 +8444,10 @@
         <v>27</v>
       </c>
       <c r="H290" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="I290" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="291" spans="1:9">
@@ -8428,13 +8467,13 @@
         <v>22</v>
       </c>
       <c r="F291" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H291" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="I291" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="292" spans="1:9">
@@ -8454,13 +8493,13 @@
         <v>26</v>
       </c>
       <c r="F292" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="H292" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="I292" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="293" spans="1:9">
@@ -8480,10 +8519,10 @@
         <v>112</v>
       </c>
       <c r="H293" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="I293" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="294" spans="1:9">
@@ -8503,13 +8542,13 @@
         <v>22</v>
       </c>
       <c r="F294" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="H294" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="I294" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="295" spans="1:9">
@@ -8529,7 +8568,7 @@
         <v>41</v>
       </c>
       <c r="F295" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="296" spans="1:9">
@@ -8549,7 +8588,7 @@
         <v>33</v>
       </c>
       <c r="F296" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="297" spans="1:9">
@@ -8569,13 +8608,13 @@
         <v>41</v>
       </c>
       <c r="F297" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="H297" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="I297" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="298" spans="1:9">
@@ -8612,10 +8651,10 @@
         <v>22</v>
       </c>
       <c r="H299" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="I299" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="300" spans="1:9">
@@ -8635,13 +8674,13 @@
         <v>22</v>
       </c>
       <c r="F300" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H300" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="I300" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="301" spans="1:9">
@@ -8661,13 +8700,13 @@
         <v>22</v>
       </c>
       <c r="F301" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="H301" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="I301" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="302" spans="1:9">
@@ -8687,10 +8726,10 @@
         <v>114</v>
       </c>
       <c r="H302" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="I302" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="303" spans="1:9">
@@ -8710,10 +8749,10 @@
         <v>115</v>
       </c>
       <c r="H303" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="I303" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="304" spans="1:9">
@@ -8733,10 +8772,10 @@
         <v>54</v>
       </c>
       <c r="H304" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="I304" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="305" spans="1:9">
@@ -8756,10 +8795,10 @@
         <v>116</v>
       </c>
       <c r="H305" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="I305" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="306" spans="1:9">
@@ -8779,10 +8818,10 @@
         <v>117</v>
       </c>
       <c r="H306" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="I306" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="307" spans="1:9">
@@ -8802,13 +8841,13 @@
         <v>22</v>
       </c>
       <c r="F307" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H307" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="I307" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="308" spans="1:9">
@@ -8828,10 +8867,10 @@
         <v>118</v>
       </c>
       <c r="H308" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="I308" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="309" spans="1:9">
@@ -8851,13 +8890,13 @@
         <v>22</v>
       </c>
       <c r="F309" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H309" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="I309" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="310" spans="1:9">
@@ -8877,10 +8916,10 @@
         <v>119</v>
       </c>
       <c r="H310" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="I310" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="311" spans="1:9">
@@ -8900,10 +8939,10 @@
         <v>55</v>
       </c>
       <c r="H311" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="I311" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="312" spans="1:9">
@@ -8923,10 +8962,10 @@
         <v>31</v>
       </c>
       <c r="H312" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="I312" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="313" spans="1:9">
@@ -8946,10 +8985,10 @@
         <v>55</v>
       </c>
       <c r="H313" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="I313" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="314" spans="1:9">
@@ -8969,13 +9008,13 @@
         <v>22</v>
       </c>
       <c r="F314" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H314" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="I314" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="315" spans="1:9">
@@ -8995,10 +9034,10 @@
         <v>120</v>
       </c>
       <c r="H315" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="I315" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="316" spans="1:9">
@@ -9018,10 +9057,10 @@
         <v>26</v>
       </c>
       <c r="F316" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="H316" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
     </row>
     <row r="317" spans="1:9">
@@ -9041,10 +9080,10 @@
         <v>121</v>
       </c>
       <c r="H317" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="I317" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="318" spans="1:9">
@@ -9064,10 +9103,10 @@
         <v>58</v>
       </c>
       <c r="H318" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="I318" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="319" spans="1:9">
@@ -9087,10 +9126,10 @@
         <v>55</v>
       </c>
       <c r="H319" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="I319" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="320" spans="1:9">
@@ -9110,10 +9149,10 @@
         <v>122</v>
       </c>
       <c r="H320" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="I320" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="321" spans="1:9">
@@ -9133,13 +9172,13 @@
         <v>22</v>
       </c>
       <c r="F321" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="H321" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="I321" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="322" spans="1:9">
@@ -9159,13 +9198,13 @@
         <v>22</v>
       </c>
       <c r="F322" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H322" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="I322" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="323" spans="1:9">
@@ -9185,13 +9224,13 @@
         <v>28</v>
       </c>
       <c r="F323" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="H323" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="I323" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
     </row>
     <row r="324" spans="1:9">
@@ -9211,10 +9250,10 @@
         <v>123</v>
       </c>
       <c r="H324" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="I324" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="325" spans="1:9">
@@ -9234,10 +9273,10 @@
         <v>55</v>
       </c>
       <c r="H325" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="I325" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="326" spans="1:9">
@@ -9257,13 +9296,13 @@
         <v>22</v>
       </c>
       <c r="F326" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="H326" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="I326" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="327" spans="1:9">
@@ -9283,13 +9322,13 @@
         <v>22</v>
       </c>
       <c r="F327" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H327" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="I327" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
     </row>
     <row r="328" spans="1:9">
@@ -9309,10 +9348,229 @@
         <v>54</v>
       </c>
       <c r="H328" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="I328" t="s">
-        <v>450</v>
+        <v>463</v>
+      </c>
+    </row>
+    <row r="329" spans="1:9">
+      <c r="A329" s="1">
+        <v>327</v>
+      </c>
+      <c r="B329" s="2">
+        <v>42794</v>
+      </c>
+      <c r="C329" t="s">
+        <v>9</v>
+      </c>
+      <c r="D329" t="s">
+        <v>18</v>
+      </c>
+      <c r="E329" t="s">
+        <v>124</v>
+      </c>
+      <c r="H329" t="s">
+        <v>454</v>
+      </c>
+      <c r="I329" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="330" spans="1:9">
+      <c r="A330" s="1">
+        <v>328</v>
+      </c>
+      <c r="B330" s="2">
+        <v>42793</v>
+      </c>
+      <c r="C330" t="s">
+        <v>9</v>
+      </c>
+      <c r="D330" t="s">
+        <v>17</v>
+      </c>
+      <c r="E330" t="s">
+        <v>22</v>
+      </c>
+      <c r="F330" t="s">
+        <v>186</v>
+      </c>
+      <c r="H330" t="s">
+        <v>455</v>
+      </c>
+      <c r="I330" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="331" spans="1:9">
+      <c r="A331" s="1">
+        <v>329</v>
+      </c>
+      <c r="B331" s="2">
+        <v>42797</v>
+      </c>
+      <c r="C331" t="s">
+        <v>9</v>
+      </c>
+      <c r="D331" t="s">
+        <v>17</v>
+      </c>
+      <c r="E331" t="s">
+        <v>22</v>
+      </c>
+      <c r="F331" t="s">
+        <v>186</v>
+      </c>
+      <c r="H331" t="s">
+        <v>456</v>
+      </c>
+      <c r="I331" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="332" spans="1:9">
+      <c r="A332" s="1">
+        <v>330</v>
+      </c>
+      <c r="B332" s="2">
+        <v>42799</v>
+      </c>
+      <c r="C332" t="s">
+        <v>9</v>
+      </c>
+      <c r="D332" t="s">
+        <v>17</v>
+      </c>
+      <c r="E332" t="s">
+        <v>22</v>
+      </c>
+      <c r="F332" t="s">
+        <v>148</v>
+      </c>
+      <c r="H332" t="s">
+        <v>457</v>
+      </c>
+      <c r="I332" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="333" spans="1:9">
+      <c r="A333" s="1">
+        <v>331</v>
+      </c>
+      <c r="B333" s="2">
+        <v>42799</v>
+      </c>
+      <c r="C333" t="s">
+        <v>9</v>
+      </c>
+      <c r="D333" t="s">
+        <v>17</v>
+      </c>
+      <c r="E333" t="s">
+        <v>23</v>
+      </c>
+      <c r="H333" t="s">
+        <v>458</v>
+      </c>
+      <c r="I333" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="334" spans="1:9">
+      <c r="A334" s="1">
+        <v>332</v>
+      </c>
+      <c r="B334" s="2">
+        <v>42801</v>
+      </c>
+      <c r="C334" t="s">
+        <v>9</v>
+      </c>
+      <c r="D334" t="s">
+        <v>19</v>
+      </c>
+      <c r="E334" t="s">
+        <v>125</v>
+      </c>
+      <c r="H334" t="s">
+        <v>459</v>
+      </c>
+      <c r="I334" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="335" spans="1:9">
+      <c r="A335" s="1">
+        <v>333</v>
+      </c>
+      <c r="B335" s="2">
+        <v>42801</v>
+      </c>
+      <c r="C335" t="s">
+        <v>9</v>
+      </c>
+      <c r="D335" t="s">
+        <v>16</v>
+      </c>
+      <c r="E335" t="s">
+        <v>58</v>
+      </c>
+      <c r="H335" t="s">
+        <v>460</v>
+      </c>
+      <c r="I335" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="336" spans="1:9">
+      <c r="A336" s="1">
+        <v>334</v>
+      </c>
+      <c r="B336" s="2">
+        <v>42800</v>
+      </c>
+      <c r="C336" t="s">
+        <v>9</v>
+      </c>
+      <c r="D336" t="s">
+        <v>17</v>
+      </c>
+      <c r="E336" t="s">
+        <v>91</v>
+      </c>
+      <c r="F336" t="s">
+        <v>204</v>
+      </c>
+      <c r="H336" t="s">
+        <v>461</v>
+      </c>
+      <c r="I336" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="337" spans="1:9">
+      <c r="A337" s="1">
+        <v>335</v>
+      </c>
+      <c r="B337" s="2">
+        <v>42804</v>
+      </c>
+      <c r="C337" t="s">
+        <v>9</v>
+      </c>
+      <c r="D337" t="s">
+        <v>18</v>
+      </c>
+      <c r="E337" t="s">
+        <v>126</v>
+      </c>
+      <c r="H337" t="s">
+        <v>462</v>
+      </c>
+      <c r="I337" t="s">
+        <v>463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating folder structure and feedback plots
</commit_message>
<xml_diff>
--- a/xlsx/OTP_feedback_tracking_cleaned_no_pi.xlsx
+++ b/xlsx/OTP_feedback_tracking_cleaned_no_pi.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="475">
   <si>
     <t>Date Received</t>
   </si>
@@ -397,6 +397,12 @@
     <t>"Thanks again"</t>
   </si>
   <si>
+    <t>Unhappy with trip plan; Confused by route map</t>
+  </si>
+  <si>
+    <t>Thinks trip plan is incorrect</t>
+  </si>
+  <si>
     <t>Location outside district</t>
   </si>
   <si>
@@ -631,6 +637,9 @@
     <t>Routed on footway that is too rough to use</t>
   </si>
   <si>
+    <t>User accidentally selected PM instead of AM</t>
+  </si>
+  <si>
     <t>Vancouver</t>
   </si>
   <si>
@@ -1403,6 +1412,24 @@
   </si>
   <si>
     <t>https://trimet.org/#planner/results/from=3508+NE+BROADWAY%2C+Portland%3A%3A45.53481%2C-122.628&amp;to=3911+SE+MILWAUKIE+AVE%2C+Portland%3A%3A45.494194%2C-122.65303</t>
+  </si>
+  <si>
+    <t>https://trimet.org/schedules/img/017.png</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#/planner/results/itin_num=3&amp;from=Current</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#/planner/results/itin_num=1&amp;from=930%20NW%20NAITO%20PKWY,%20Portland::45.529015,-122.673416&amp;to=Benson%20Polytechnic%20High,%20Portland::45.527313,-122.65263&amp;Walk=1260&amp;Arr=D</t>
+  </si>
+  <si>
+    <t>http://trimet.org/#planner/results/from=SW+ALLEN+BLVD+%26+SW+HALL+BLVD%3A%3A45.476464%2C-122.805481&amp;to=11361+SW+LEVETON+DR%3A%3A45.386046%2C-122.794318&amp;m=pm&amp;walk=1260&amp;arr=A</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=1511+SW+PARK+AVE%2C+Portland%3A%3A45.514206%2C-122.68472&amp;to=631+NE+102ND+AVE%2C+Portland%3A%3A45.527378%2C-122.55855&amp;m=pm&amp;walk=1260&amp;optimize=TRANSFERS&amp;arr=A</t>
+  </si>
+  <si>
+    <t>https://trimet.org/#planner/results/from=187+SE+18TH+AVE%2C+Hillsboro%3A%3A45.521034%2C-122.96407&amp;to=6360+SE+ALEXANDER+ST%2C+Hillsboro%3A%3A45.496017%2C-122.916664&amp;m=pm&amp;walk=1260&amp;arr=A</t>
   </si>
   <si>
     <t>Weekday</t>
@@ -1773,7 +1800,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I337"/>
+  <dimension ref="A1:I343"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1869,13 +1896,13 @@
         <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G4" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="H4" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1895,13 +1922,13 @@
         <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G5" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="H5" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1921,10 +1948,10 @@
         <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="I6" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1984,7 +2011,7 @@
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2004,13 +2031,13 @@
         <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G10" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="H10" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2047,13 +2074,13 @@
         <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G12" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="H12" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2073,7 +2100,7 @@
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2093,7 +2120,7 @@
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2133,13 +2160,13 @@
         <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G16" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="H16" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2176,7 +2203,7 @@
         <v>22</v>
       </c>
       <c r="F18" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2196,10 +2223,10 @@
         <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H19" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2219,13 +2246,13 @@
         <v>23</v>
       </c>
       <c r="F20" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G20" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="H20" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2245,10 +2272,10 @@
         <v>26</v>
       </c>
       <c r="F21" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H21" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2268,13 +2295,13 @@
         <v>23</v>
       </c>
       <c r="F22" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G22" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="H22" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2294,13 +2321,13 @@
         <v>23</v>
       </c>
       <c r="F23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G23" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="H23" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2320,7 +2347,7 @@
         <v>22</v>
       </c>
       <c r="F24" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2357,7 +2384,7 @@
         <v>33</v>
       </c>
       <c r="F26" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2377,10 +2404,10 @@
         <v>26</v>
       </c>
       <c r="F27" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H27" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2400,10 +2427,10 @@
         <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H28" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2423,13 +2450,13 @@
         <v>23</v>
       </c>
       <c r="F29" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G29" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="H29" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2449,13 +2476,13 @@
         <v>23</v>
       </c>
       <c r="F30" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G30" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="H30" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2492,13 +2519,13 @@
         <v>23</v>
       </c>
       <c r="F32" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G32" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="H32" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2518,10 +2545,10 @@
         <v>26</v>
       </c>
       <c r="F33" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H33" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2558,10 +2585,10 @@
         <v>23</v>
       </c>
       <c r="F35" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G35" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2581,10 +2608,10 @@
         <v>23</v>
       </c>
       <c r="F36" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G36" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2604,10 +2631,10 @@
         <v>26</v>
       </c>
       <c r="F37" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H37" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2661,10 +2688,10 @@
         <v>26</v>
       </c>
       <c r="F40" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H40" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2684,13 +2711,13 @@
         <v>23</v>
       </c>
       <c r="F41" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G41" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="H41" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2710,13 +2737,13 @@
         <v>23</v>
       </c>
       <c r="F42" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G42" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="H42" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2736,7 +2763,7 @@
         <v>37</v>
       </c>
       <c r="F43" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2756,10 +2783,10 @@
         <v>26</v>
       </c>
       <c r="F44" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H44" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2779,10 +2806,10 @@
         <v>26</v>
       </c>
       <c r="F45" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H45" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2802,7 +2829,7 @@
         <v>22</v>
       </c>
       <c r="F46" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2822,10 +2849,10 @@
         <v>26</v>
       </c>
       <c r="F47" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H47" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2862,10 +2889,10 @@
         <v>26</v>
       </c>
       <c r="F49" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H49" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2885,7 +2912,7 @@
         <v>22</v>
       </c>
       <c r="F50" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2962,13 +2989,13 @@
         <v>23</v>
       </c>
       <c r="F54" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G54" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="H54" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2988,10 +3015,10 @@
         <v>26</v>
       </c>
       <c r="F55" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H55" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -3065,7 +3092,7 @@
         <v>41</v>
       </c>
       <c r="F59" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -3085,7 +3112,7 @@
         <v>41</v>
       </c>
       <c r="F60" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -3142,13 +3169,13 @@
         <v>23</v>
       </c>
       <c r="F63" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G63" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="H63" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -3168,10 +3195,10 @@
         <v>44</v>
       </c>
       <c r="H64" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="I64" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -3191,10 +3218,10 @@
         <v>45</v>
       </c>
       <c r="H65" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="I65" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -3231,7 +3258,7 @@
         <v>26</v>
       </c>
       <c r="F67" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -3251,13 +3278,13 @@
         <v>46</v>
       </c>
       <c r="F68" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H68" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="I68" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -3277,13 +3304,13 @@
         <v>22</v>
       </c>
       <c r="F69" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H69" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="I69" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -3323,10 +3350,10 @@
         <v>44</v>
       </c>
       <c r="H71" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="I71" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -3346,13 +3373,13 @@
         <v>47</v>
       </c>
       <c r="F72" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="H72" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="I72" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -3372,13 +3399,13 @@
         <v>47</v>
       </c>
       <c r="F73" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H73" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="I73" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -3398,7 +3425,7 @@
         <v>22</v>
       </c>
       <c r="F74" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -3418,10 +3445,10 @@
         <v>48</v>
       </c>
       <c r="H75" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="I75" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -3441,10 +3468,10 @@
         <v>49</v>
       </c>
       <c r="H76" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="I76" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -3464,10 +3491,10 @@
         <v>50</v>
       </c>
       <c r="H77" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="I77" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -3504,10 +3531,10 @@
         <v>52</v>
       </c>
       <c r="H79" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="I79" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -3527,10 +3554,10 @@
         <v>21</v>
       </c>
       <c r="H80" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="I80" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -3553,10 +3580,10 @@
         <v>20</v>
       </c>
       <c r="H81" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="I81" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -3576,10 +3603,10 @@
         <v>53</v>
       </c>
       <c r="H82" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="I82" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3599,10 +3626,10 @@
         <v>54</v>
       </c>
       <c r="H83" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="I83" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -3622,10 +3649,10 @@
         <v>31</v>
       </c>
       <c r="H84" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="I84" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -3645,10 +3672,10 @@
         <v>55</v>
       </c>
       <c r="H85" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="I85" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -3668,10 +3695,10 @@
         <v>56</v>
       </c>
       <c r="H86" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="I86" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -3694,10 +3721,10 @@
         <v>20</v>
       </c>
       <c r="H87" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="I87" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -3717,13 +3744,13 @@
         <v>22</v>
       </c>
       <c r="F88" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H88" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="I88" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -3746,10 +3773,10 @@
         <v>20</v>
       </c>
       <c r="H89" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="I89" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -3769,10 +3796,10 @@
         <v>58</v>
       </c>
       <c r="H90" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="I90" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3792,7 +3819,7 @@
         <v>22</v>
       </c>
       <c r="F91" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -3852,10 +3879,10 @@
         <v>20</v>
       </c>
       <c r="H94" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="I94" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -3875,13 +3902,13 @@
         <v>22</v>
       </c>
       <c r="F95" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H95" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="I95" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -3901,13 +3928,13 @@
         <v>22</v>
       </c>
       <c r="F96" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H96" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="I96" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -3927,13 +3954,13 @@
         <v>60</v>
       </c>
       <c r="F97" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H97" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="I97" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -3953,10 +3980,10 @@
         <v>61</v>
       </c>
       <c r="H98" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="I98" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -3976,13 +4003,13 @@
         <v>22</v>
       </c>
       <c r="F99" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H99" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="I99" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -4002,10 +4029,10 @@
         <v>54</v>
       </c>
       <c r="H100" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="I100" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -4025,7 +4052,7 @@
         <v>28</v>
       </c>
       <c r="F101" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -4045,10 +4072,10 @@
         <v>54</v>
       </c>
       <c r="H102" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="I102" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -4068,13 +4095,13 @@
         <v>62</v>
       </c>
       <c r="F103" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H103" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="I103" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -4094,13 +4121,13 @@
         <v>62</v>
       </c>
       <c r="F104" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H104" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="I104" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -4120,10 +4147,10 @@
         <v>35</v>
       </c>
       <c r="H105" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="I105" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -4143,13 +4170,13 @@
         <v>62</v>
       </c>
       <c r="F106" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H106" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="I106" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -4169,13 +4196,13 @@
         <v>41</v>
       </c>
       <c r="F107" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H107" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="I107" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -4195,13 +4222,13 @@
         <v>22</v>
       </c>
       <c r="F108" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H108" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="I108" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -4221,13 +4248,13 @@
         <v>22</v>
       </c>
       <c r="F109" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H109" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="I109" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -4247,10 +4274,10 @@
         <v>31</v>
       </c>
       <c r="H110" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="I110" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -4270,10 +4297,10 @@
         <v>23</v>
       </c>
       <c r="H111" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="I111" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -4293,7 +4320,7 @@
         <v>26</v>
       </c>
       <c r="F112" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="113" spans="1:9">
@@ -4313,10 +4340,10 @@
         <v>44</v>
       </c>
       <c r="H113" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="I113" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -4353,13 +4380,13 @@
         <v>64</v>
       </c>
       <c r="F115" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H115" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="I115" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
     </row>
     <row r="116" spans="1:9">
@@ -4396,7 +4423,7 @@
         <v>66</v>
       </c>
       <c r="H117" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="118" spans="1:9">
@@ -4416,10 +4443,10 @@
         <v>45</v>
       </c>
       <c r="H118" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="I118" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="119" spans="1:9">
@@ -4456,10 +4483,10 @@
         <v>67</v>
       </c>
       <c r="H120" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="I120" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="121" spans="1:9">
@@ -4479,7 +4506,7 @@
         <v>22</v>
       </c>
       <c r="F121" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="122" spans="1:9">
@@ -4519,10 +4546,10 @@
         <v>20</v>
       </c>
       <c r="H123" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="I123" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="124" spans="1:9">
@@ -4542,10 +4569,10 @@
         <v>69</v>
       </c>
       <c r="H124" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="I124" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="125" spans="1:9">
@@ -4565,13 +4592,13 @@
         <v>26</v>
       </c>
       <c r="F125" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H125" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="I125" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="126" spans="1:9">
@@ -4591,10 +4618,10 @@
         <v>35</v>
       </c>
       <c r="H126" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="I126" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="127" spans="1:9">
@@ -4631,10 +4658,10 @@
         <v>27</v>
       </c>
       <c r="H128" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="I128" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="129" spans="1:9">
@@ -4654,13 +4681,13 @@
         <v>22</v>
       </c>
       <c r="F129" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H129" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="I129" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -4680,10 +4707,10 @@
         <v>70</v>
       </c>
       <c r="H130" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="I130" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="131" spans="1:9">
@@ -4703,10 +4730,10 @@
         <v>71</v>
       </c>
       <c r="H131" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="I131" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="132" spans="1:9">
@@ -4726,13 +4753,13 @@
         <v>22</v>
       </c>
       <c r="F132" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H132" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="I132" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="133" spans="1:9">
@@ -4752,10 +4779,10 @@
         <v>26</v>
       </c>
       <c r="F133" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="H133" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="134" spans="1:9">
@@ -4775,7 +4802,7 @@
         <v>33</v>
       </c>
       <c r="F134" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="135" spans="1:9">
@@ -4815,10 +4842,10 @@
         <v>54</v>
       </c>
       <c r="H136" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="I136" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="137" spans="1:9">
@@ -4838,13 +4865,13 @@
         <v>72</v>
       </c>
       <c r="F137" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H137" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="I137" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="138" spans="1:9">
@@ -4864,10 +4891,10 @@
         <v>26</v>
       </c>
       <c r="F138" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H138" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="139" spans="1:9">
@@ -4887,10 +4914,10 @@
         <v>26</v>
       </c>
       <c r="F139" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H139" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="140" spans="1:9">
@@ -4910,13 +4937,13 @@
         <v>73</v>
       </c>
       <c r="F140" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H140" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="I140" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="141" spans="1:9">
@@ -4936,13 +4963,13 @@
         <v>22</v>
       </c>
       <c r="F141" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H141" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="I141" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="142" spans="1:9">
@@ -4982,10 +5009,10 @@
         <v>68</v>
       </c>
       <c r="H143" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="I143" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -5005,10 +5032,10 @@
         <v>52</v>
       </c>
       <c r="H144" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="I144" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -5028,10 +5055,10 @@
         <v>21</v>
       </c>
       <c r="H145" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="I145" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -5051,13 +5078,13 @@
         <v>22</v>
       </c>
       <c r="F146" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H146" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="I146" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -5077,10 +5104,10 @@
         <v>26</v>
       </c>
       <c r="F147" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H147" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -5100,10 +5127,10 @@
         <v>33</v>
       </c>
       <c r="F148" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H148" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -5123,7 +5150,7 @@
         <v>33</v>
       </c>
       <c r="F149" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -5143,7 +5170,7 @@
         <v>22</v>
       </c>
       <c r="F150" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -5163,13 +5190,13 @@
         <v>22</v>
       </c>
       <c r="F151" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H151" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="I151" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -5189,13 +5216,13 @@
         <v>22</v>
       </c>
       <c r="F152" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H152" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="I152" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -5215,13 +5242,13 @@
         <v>41</v>
       </c>
       <c r="F153" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H153" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="I153" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="154" spans="1:9">
@@ -5241,7 +5268,7 @@
         <v>26</v>
       </c>
       <c r="F154" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -5261,13 +5288,13 @@
         <v>22</v>
       </c>
       <c r="F155" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H155" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="I155" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="156" spans="1:9">
@@ -5287,10 +5314,10 @@
         <v>74</v>
       </c>
       <c r="H156" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="I156" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="157" spans="1:9">
@@ -5310,10 +5337,10 @@
         <v>75</v>
       </c>
       <c r="H157" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="I157" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="158" spans="1:9">
@@ -5350,13 +5377,13 @@
         <v>76</v>
       </c>
       <c r="F159" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H159" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="I159" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="160" spans="1:9">
@@ -5376,10 +5403,10 @@
         <v>77</v>
       </c>
       <c r="H160" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="I160" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="161" spans="1:9">
@@ -5399,13 +5426,13 @@
         <v>22</v>
       </c>
       <c r="F161" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H161" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="I161" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="162" spans="1:9">
@@ -5425,10 +5452,10 @@
         <v>78</v>
       </c>
       <c r="H162" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="I162" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="163" spans="1:9">
@@ -5448,13 +5475,13 @@
         <v>22</v>
       </c>
       <c r="F163" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H163" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="I163" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="164" spans="1:9">
@@ -5494,7 +5521,7 @@
         <v>20</v>
       </c>
       <c r="H165" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="166" spans="1:9">
@@ -5514,13 +5541,13 @@
         <v>22</v>
       </c>
       <c r="F166" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H166" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="I166" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="167" spans="1:9">
@@ -5557,13 +5584,13 @@
         <v>23</v>
       </c>
       <c r="F168" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G168" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="H168" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="169" spans="1:9">
@@ -5583,13 +5610,13 @@
         <v>41</v>
       </c>
       <c r="F169" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H169" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="I169" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="170" spans="1:9">
@@ -5609,10 +5636,10 @@
         <v>31</v>
       </c>
       <c r="H170" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="I170" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="171" spans="1:9">
@@ -5632,10 +5659,10 @@
         <v>45</v>
       </c>
       <c r="H171" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="I171" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="172" spans="1:9">
@@ -5655,10 +5682,10 @@
         <v>81</v>
       </c>
       <c r="H172" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="I172" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="173" spans="1:9">
@@ -5678,10 +5705,10 @@
         <v>58</v>
       </c>
       <c r="H173" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="I173" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="174" spans="1:9">
@@ -5701,13 +5728,13 @@
         <v>31</v>
       </c>
       <c r="F174" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H174" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="I174" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="175" spans="1:9">
@@ -5730,10 +5757,10 @@
         <v>20</v>
       </c>
       <c r="H175" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="I175" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="176" spans="1:9">
@@ -5753,13 +5780,13 @@
         <v>22</v>
       </c>
       <c r="F176" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H176" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="I176" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="177" spans="1:9">
@@ -5779,7 +5806,7 @@
         <v>26</v>
       </c>
       <c r="F177" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="178" spans="1:9">
@@ -5799,10 +5826,10 @@
         <v>82</v>
       </c>
       <c r="H178" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="I178" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="179" spans="1:9">
@@ -5822,10 +5849,10 @@
         <v>83</v>
       </c>
       <c r="H179" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="I179" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="180" spans="1:9">
@@ -5845,13 +5872,13 @@
         <v>41</v>
       </c>
       <c r="F180" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H180" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="I180" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="181" spans="1:9">
@@ -5871,13 +5898,13 @@
         <v>41</v>
       </c>
       <c r="F181" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H181" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="I181" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="182" spans="1:9">
@@ -5900,10 +5927,10 @@
         <v>20</v>
       </c>
       <c r="H182" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="I182" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="183" spans="1:9">
@@ -5923,10 +5950,10 @@
         <v>23</v>
       </c>
       <c r="F183" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G183" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="184" spans="1:9">
@@ -5946,10 +5973,10 @@
         <v>84</v>
       </c>
       <c r="H184" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="I184" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="185" spans="1:9">
@@ -5969,7 +5996,7 @@
         <v>22</v>
       </c>
       <c r="F185" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="186" spans="1:9">
@@ -5989,10 +6016,10 @@
         <v>85</v>
       </c>
       <c r="H186" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="I186" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="187" spans="1:9">
@@ -6012,13 +6039,13 @@
         <v>86</v>
       </c>
       <c r="F187" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H187" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="I187" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="188" spans="1:9">
@@ -6038,13 +6065,13 @@
         <v>22</v>
       </c>
       <c r="F188" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="H188" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="I188" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="189" spans="1:9">
@@ -6064,10 +6091,10 @@
         <v>87</v>
       </c>
       <c r="H189" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="I189" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="190" spans="1:9">
@@ -6087,10 +6114,10 @@
         <v>20</v>
       </c>
       <c r="H190" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="I190" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="191" spans="1:9">
@@ -6110,10 +6137,10 @@
         <v>88</v>
       </c>
       <c r="F191" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H191" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="192" spans="1:9">
@@ -6133,10 +6160,10 @@
         <v>45</v>
       </c>
       <c r="H192" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="I192" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="193" spans="1:9">
@@ -6156,10 +6183,10 @@
         <v>89</v>
       </c>
       <c r="H193" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="I193" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="194" spans="1:9">
@@ -6182,10 +6209,10 @@
         <v>20</v>
       </c>
       <c r="H194" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="I194" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="195" spans="1:9">
@@ -6205,10 +6232,10 @@
         <v>21</v>
       </c>
       <c r="H195" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="I195" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="196" spans="1:9">
@@ -6228,13 +6255,13 @@
         <v>41</v>
       </c>
       <c r="F196" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H196" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="I196" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="197" spans="1:9">
@@ -6254,13 +6281,13 @@
         <v>22</v>
       </c>
       <c r="F197" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H197" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="I197" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="198" spans="1:9">
@@ -6280,10 +6307,10 @@
         <v>54</v>
       </c>
       <c r="H198" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="I198" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="199" spans="1:9">
@@ -6303,13 +6330,13 @@
         <v>22</v>
       </c>
       <c r="F199" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H199" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="I199" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="200" spans="1:9">
@@ -6329,13 +6356,13 @@
         <v>22</v>
       </c>
       <c r="F200" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H200" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="I200" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="201" spans="1:9">
@@ -6355,13 +6382,13 @@
         <v>22</v>
       </c>
       <c r="F201" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H201" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="I201" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="202" spans="1:9">
@@ -6381,13 +6408,13 @@
         <v>90</v>
       </c>
       <c r="F202" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H202" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="I202" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="203" spans="1:9">
@@ -6407,10 +6434,10 @@
         <v>55</v>
       </c>
       <c r="H203" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="I203" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="204" spans="1:9">
@@ -6430,10 +6457,10 @@
         <v>55</v>
       </c>
       <c r="H204" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="I204" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="205" spans="1:9">
@@ -6453,10 +6480,10 @@
         <v>54</v>
       </c>
       <c r="H205" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="I205" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="206" spans="1:9">
@@ -6476,10 +6503,10 @@
         <v>54</v>
       </c>
       <c r="H206" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I206" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="207" spans="1:9">
@@ -6499,10 +6526,10 @@
         <v>31</v>
       </c>
       <c r="H207" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="I207" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="208" spans="1:9">
@@ -6522,7 +6549,7 @@
         <v>91</v>
       </c>
       <c r="F208" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="209" spans="1:9">
@@ -6542,10 +6569,10 @@
         <v>92</v>
       </c>
       <c r="H209" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="I209" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="210" spans="1:9">
@@ -6565,10 +6592,10 @@
         <v>35</v>
       </c>
       <c r="H210" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="I210" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="211" spans="1:9">
@@ -6588,10 +6615,10 @@
         <v>54</v>
       </c>
       <c r="H211" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="I211" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="212" spans="1:9">
@@ -6611,13 +6638,13 @@
         <v>22</v>
       </c>
       <c r="F212" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H212" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="I212" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="213" spans="1:9">
@@ -6637,13 +6664,13 @@
         <v>22</v>
       </c>
       <c r="F213" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H213" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="I213" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="214" spans="1:9">
@@ -6663,10 +6690,10 @@
         <v>54</v>
       </c>
       <c r="H214" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="I214" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="215" spans="1:9">
@@ -6686,13 +6713,13 @@
         <v>22</v>
       </c>
       <c r="F215" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H215" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="I215" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="216" spans="1:9">
@@ -6712,10 +6739,10 @@
         <v>93</v>
       </c>
       <c r="H216" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="I216" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="217" spans="1:9">
@@ -6735,13 +6762,13 @@
         <v>94</v>
       </c>
       <c r="F217" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="H217" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="I217" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="218" spans="1:9">
@@ -6761,13 +6788,13 @@
         <v>22</v>
       </c>
       <c r="F218" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H218" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="I218" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="219" spans="1:9">
@@ -6787,13 +6814,13 @@
         <v>95</v>
       </c>
       <c r="F219" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H219" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="I219" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="220" spans="1:9">
@@ -6813,10 +6840,10 @@
         <v>31</v>
       </c>
       <c r="H220" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="I220" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="221" spans="1:9">
@@ -6836,13 +6863,13 @@
         <v>95</v>
       </c>
       <c r="F221" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H221" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="I221" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="222" spans="1:9">
@@ -6862,13 +6889,13 @@
         <v>22</v>
       </c>
       <c r="F222" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H222" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="I222" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="223" spans="1:9">
@@ -6888,13 +6915,13 @@
         <v>22</v>
       </c>
       <c r="F223" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H223" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="I223" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="224" spans="1:9">
@@ -6931,13 +6958,13 @@
         <v>95</v>
       </c>
       <c r="F225" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H225" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="I225" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="226" spans="1:9">
@@ -6974,13 +7001,13 @@
         <v>95</v>
       </c>
       <c r="F227" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H227" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="I227" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="228" spans="1:9">
@@ -7017,10 +7044,10 @@
         <v>98</v>
       </c>
       <c r="H229" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="I229" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="230" spans="1:9">
@@ -7040,13 +7067,13 @@
         <v>95</v>
       </c>
       <c r="F230" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H230" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="I230" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="231" spans="1:9">
@@ -7066,10 +7093,10 @@
         <v>99</v>
       </c>
       <c r="H231" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="I231" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="232" spans="1:9">
@@ -7123,10 +7150,10 @@
         <v>101</v>
       </c>
       <c r="H234" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="I234" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="235" spans="1:9">
@@ -7146,13 +7173,13 @@
         <v>102</v>
       </c>
       <c r="F235" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H235" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="I235" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="236" spans="1:9">
@@ -7172,13 +7199,13 @@
         <v>22</v>
       </c>
       <c r="F236" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H236" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="I236" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="237" spans="1:9">
@@ -7198,10 +7225,10 @@
         <v>103</v>
       </c>
       <c r="H237" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="I237" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="238" spans="1:9">
@@ -7221,13 +7248,13 @@
         <v>22</v>
       </c>
       <c r="F238" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H238" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="I238" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="239" spans="1:9">
@@ -7247,13 +7274,13 @@
         <v>22</v>
       </c>
       <c r="F239" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H239" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="I239" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="240" spans="1:9">
@@ -7273,10 +7300,10 @@
         <v>104</v>
       </c>
       <c r="H240" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="I240" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="241" spans="1:9">
@@ -7296,10 +7323,10 @@
         <v>45</v>
       </c>
       <c r="H241" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I241" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="242" spans="1:9">
@@ -7339,10 +7366,10 @@
         <v>58</v>
       </c>
       <c r="H243" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="I243" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="244" spans="1:9">
@@ -7362,7 +7389,7 @@
         <v>22</v>
       </c>
       <c r="F244" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="245" spans="1:9">
@@ -7382,13 +7409,13 @@
         <v>91</v>
       </c>
       <c r="F245" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H245" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="I245" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="246" spans="1:9">
@@ -7408,13 +7435,13 @@
         <v>22</v>
       </c>
       <c r="F246" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H246" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="I246" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="247" spans="1:9">
@@ -7434,10 +7461,10 @@
         <v>56</v>
       </c>
       <c r="H247" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="I247" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="248" spans="1:9">
@@ -7457,7 +7484,7 @@
         <v>41</v>
       </c>
       <c r="F248" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="249" spans="1:9">
@@ -7477,13 +7504,13 @@
         <v>22</v>
       </c>
       <c r="F249" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H249" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I249" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="250" spans="1:9">
@@ -7523,13 +7550,13 @@
         <v>22</v>
       </c>
       <c r="F251" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="H251" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="I251" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="252" spans="1:9">
@@ -7549,10 +7576,10 @@
         <v>21</v>
       </c>
       <c r="H252" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="I252" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="253" spans="1:9">
@@ -7589,10 +7616,10 @@
         <v>106</v>
       </c>
       <c r="H254" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="I254" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="255" spans="1:9">
@@ -7612,13 +7639,13 @@
         <v>22</v>
       </c>
       <c r="F255" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H255" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="I255" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="256" spans="1:9">
@@ -7638,10 +7665,10 @@
         <v>107</v>
       </c>
       <c r="H256" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="I256" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="257" spans="1:9">
@@ -7661,13 +7688,13 @@
         <v>22</v>
       </c>
       <c r="F257" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H257" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="I257" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="258" spans="1:9">
@@ -7687,13 +7714,13 @@
         <v>22</v>
       </c>
       <c r="F258" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H258" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="I258" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="259" spans="1:9">
@@ -7713,10 +7740,10 @@
         <v>108</v>
       </c>
       <c r="H259" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="I259" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="260" spans="1:9">
@@ -7736,7 +7763,7 @@
         <v>26</v>
       </c>
       <c r="F260" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="261" spans="1:9">
@@ -7756,13 +7783,13 @@
         <v>22</v>
       </c>
       <c r="F261" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H261" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="I261" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="262" spans="1:9">
@@ -7782,13 +7809,13 @@
         <v>22</v>
       </c>
       <c r="F262" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H262" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="I262" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="263" spans="1:9">
@@ -7808,10 +7835,10 @@
         <v>109</v>
       </c>
       <c r="H263" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="I263" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="264" spans="1:9">
@@ -7831,10 +7858,10 @@
         <v>31</v>
       </c>
       <c r="H264" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="I264" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="265" spans="1:9">
@@ -7854,10 +7881,10 @@
         <v>31</v>
       </c>
       <c r="H265" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="I265" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="266" spans="1:9">
@@ -7877,10 +7904,10 @@
         <v>31</v>
       </c>
       <c r="H266" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="I266" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="267" spans="1:9">
@@ -7900,13 +7927,13 @@
         <v>88</v>
       </c>
       <c r="F267" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H267" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="I267" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="268" spans="1:9">
@@ -7926,10 +7953,10 @@
         <v>31</v>
       </c>
       <c r="H268" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="I268" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="269" spans="1:9">
@@ -7949,10 +7976,10 @@
         <v>31</v>
       </c>
       <c r="H269" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="I269" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="270" spans="1:9">
@@ -7972,10 +7999,10 @@
         <v>31</v>
       </c>
       <c r="H270" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="I270" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="271" spans="1:9">
@@ -7995,10 +8022,10 @@
         <v>31</v>
       </c>
       <c r="H271" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="I271" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="272" spans="1:9">
@@ -8018,13 +8045,13 @@
         <v>22</v>
       </c>
       <c r="F272" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H272" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="I272" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="273" spans="1:9">
@@ -8044,13 +8071,13 @@
         <v>22</v>
       </c>
       <c r="F273" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H273" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="I273" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="274" spans="1:9">
@@ -8090,13 +8117,13 @@
         <v>41</v>
       </c>
       <c r="F275" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="H275" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="I275" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="276" spans="1:9">
@@ -8116,13 +8143,13 @@
         <v>22</v>
       </c>
       <c r="F276" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H276" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="I276" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="277" spans="1:9">
@@ -8142,10 +8169,10 @@
         <v>31</v>
       </c>
       <c r="H277" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="I277" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="278" spans="1:9">
@@ -8165,10 +8192,10 @@
         <v>31</v>
       </c>
       <c r="H278" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="I278" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="279" spans="1:9">
@@ -8188,10 +8215,10 @@
         <v>58</v>
       </c>
       <c r="H279" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="I279" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="280" spans="1:9">
@@ -8211,13 +8238,13 @@
         <v>22</v>
       </c>
       <c r="F280" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H280" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="I280" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="281" spans="1:9">
@@ -8237,13 +8264,13 @@
         <v>22</v>
       </c>
       <c r="F281" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H281" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="I281" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="282" spans="1:9">
@@ -8263,10 +8290,10 @@
         <v>31</v>
       </c>
       <c r="H282" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="I282" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="283" spans="1:9">
@@ -8286,13 +8313,13 @@
         <v>22</v>
       </c>
       <c r="F283" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H283" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="I283" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="284" spans="1:9">
@@ -8312,10 +8339,10 @@
         <v>31</v>
       </c>
       <c r="H284" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="I284" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="285" spans="1:9">
@@ -8335,10 +8362,10 @@
         <v>31</v>
       </c>
       <c r="H285" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="I285" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="286" spans="1:9">
@@ -8358,10 +8385,10 @@
         <v>31</v>
       </c>
       <c r="H286" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="I286" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="287" spans="1:9">
@@ -8381,10 +8408,10 @@
         <v>31</v>
       </c>
       <c r="H287" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="I287" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="288" spans="1:9">
@@ -8404,10 +8431,10 @@
         <v>110</v>
       </c>
       <c r="H288" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="I288" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="289" spans="1:9">
@@ -8444,10 +8471,10 @@
         <v>27</v>
       </c>
       <c r="H290" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="I290" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="291" spans="1:9">
@@ -8467,13 +8494,13 @@
         <v>22</v>
       </c>
       <c r="F291" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H291" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="I291" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="292" spans="1:9">
@@ -8493,13 +8520,13 @@
         <v>26</v>
       </c>
       <c r="F292" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H292" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="I292" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="293" spans="1:9">
@@ -8519,10 +8546,10 @@
         <v>112</v>
       </c>
       <c r="H293" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="I293" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="294" spans="1:9">
@@ -8542,13 +8569,13 @@
         <v>22</v>
       </c>
       <c r="F294" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H294" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="I294" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="295" spans="1:9">
@@ -8568,7 +8595,7 @@
         <v>41</v>
       </c>
       <c r="F295" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="296" spans="1:9">
@@ -8588,7 +8615,7 @@
         <v>33</v>
       </c>
       <c r="F296" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="297" spans="1:9">
@@ -8608,13 +8635,13 @@
         <v>41</v>
       </c>
       <c r="F297" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H297" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="I297" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="298" spans="1:9">
@@ -8651,10 +8678,10 @@
         <v>22</v>
       </c>
       <c r="H299" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="I299" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="300" spans="1:9">
@@ -8674,13 +8701,13 @@
         <v>22</v>
       </c>
       <c r="F300" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H300" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="I300" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="301" spans="1:9">
@@ -8700,13 +8727,13 @@
         <v>22</v>
       </c>
       <c r="F301" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="H301" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="I301" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="302" spans="1:9">
@@ -8726,10 +8753,10 @@
         <v>114</v>
       </c>
       <c r="H302" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="I302" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="303" spans="1:9">
@@ -8749,10 +8776,10 @@
         <v>115</v>
       </c>
       <c r="H303" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="I303" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="304" spans="1:9">
@@ -8772,10 +8799,10 @@
         <v>54</v>
       </c>
       <c r="H304" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="I304" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="305" spans="1:9">
@@ -8795,10 +8822,10 @@
         <v>116</v>
       </c>
       <c r="H305" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="I305" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="306" spans="1:9">
@@ -8818,10 +8845,10 @@
         <v>117</v>
       </c>
       <c r="H306" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="I306" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="307" spans="1:9">
@@ -8841,13 +8868,13 @@
         <v>22</v>
       </c>
       <c r="F307" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H307" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="I307" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="308" spans="1:9">
@@ -8867,10 +8894,10 @@
         <v>118</v>
       </c>
       <c r="H308" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="I308" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="309" spans="1:9">
@@ -8890,13 +8917,13 @@
         <v>22</v>
       </c>
       <c r="F309" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H309" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="I309" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="310" spans="1:9">
@@ -8916,10 +8943,10 @@
         <v>119</v>
       </c>
       <c r="H310" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="I310" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="311" spans="1:9">
@@ -8939,10 +8966,10 @@
         <v>55</v>
       </c>
       <c r="H311" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="I311" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="312" spans="1:9">
@@ -8962,10 +8989,10 @@
         <v>31</v>
       </c>
       <c r="H312" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="I312" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="313" spans="1:9">
@@ -8985,10 +9012,10 @@
         <v>55</v>
       </c>
       <c r="H313" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="I313" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="314" spans="1:9">
@@ -9008,13 +9035,13 @@
         <v>22</v>
       </c>
       <c r="F314" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H314" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="I314" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="315" spans="1:9">
@@ -9034,10 +9061,10 @@
         <v>120</v>
       </c>
       <c r="H315" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="I315" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="316" spans="1:9">
@@ -9057,10 +9084,10 @@
         <v>26</v>
       </c>
       <c r="F316" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H316" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="317" spans="1:9">
@@ -9080,10 +9107,10 @@
         <v>121</v>
       </c>
       <c r="H317" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="I317" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="318" spans="1:9">
@@ -9103,10 +9130,10 @@
         <v>58</v>
       </c>
       <c r="H318" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="I318" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="319" spans="1:9">
@@ -9126,10 +9153,10 @@
         <v>55</v>
       </c>
       <c r="H319" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="I319" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="320" spans="1:9">
@@ -9149,10 +9176,10 @@
         <v>122</v>
       </c>
       <c r="H320" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="I320" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="321" spans="1:9">
@@ -9172,13 +9199,13 @@
         <v>22</v>
       </c>
       <c r="F321" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="H321" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="I321" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="322" spans="1:9">
@@ -9198,13 +9225,13 @@
         <v>22</v>
       </c>
       <c r="F322" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H322" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="I322" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="323" spans="1:9">
@@ -9224,13 +9251,13 @@
         <v>28</v>
       </c>
       <c r="F323" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H323" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="I323" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="324" spans="1:9">
@@ -9250,10 +9277,10 @@
         <v>123</v>
       </c>
       <c r="H324" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="I324" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="325" spans="1:9">
@@ -9273,10 +9300,10 @@
         <v>55</v>
       </c>
       <c r="H325" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="I325" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="326" spans="1:9">
@@ -9296,13 +9323,13 @@
         <v>22</v>
       </c>
       <c r="F326" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H326" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="I326" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="327" spans="1:9">
@@ -9322,13 +9349,13 @@
         <v>22</v>
       </c>
       <c r="F327" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H327" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="I327" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="328" spans="1:9">
@@ -9348,10 +9375,10 @@
         <v>54</v>
       </c>
       <c r="H328" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="I328" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="329" spans="1:9">
@@ -9371,10 +9398,10 @@
         <v>124</v>
       </c>
       <c r="H329" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="I329" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="330" spans="1:9">
@@ -9394,13 +9421,13 @@
         <v>22</v>
       </c>
       <c r="F330" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H330" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="I330" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="331" spans="1:9">
@@ -9420,13 +9447,13 @@
         <v>22</v>
       </c>
       <c r="F331" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H331" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="I331" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="332" spans="1:9">
@@ -9446,13 +9473,13 @@
         <v>22</v>
       </c>
       <c r="F332" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H332" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="I332" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="333" spans="1:9">
@@ -9472,10 +9499,10 @@
         <v>23</v>
       </c>
       <c r="H333" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="I333" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="334" spans="1:9">
@@ -9495,10 +9522,10 @@
         <v>125</v>
       </c>
       <c r="H334" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="I334" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="335" spans="1:9">
@@ -9518,10 +9545,10 @@
         <v>58</v>
       </c>
       <c r="H335" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="I335" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="336" spans="1:9">
@@ -9541,13 +9568,13 @@
         <v>91</v>
       </c>
       <c r="F336" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="H336" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="I336" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="337" spans="1:9">
@@ -9567,10 +9594,160 @@
         <v>126</v>
       </c>
       <c r="H337" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="I337" t="s">
-        <v>463</v>
+        <v>472</v>
+      </c>
+    </row>
+    <row r="338" spans="1:9">
+      <c r="A338" s="1">
+        <v>336</v>
+      </c>
+      <c r="B338" s="2">
+        <v>42807</v>
+      </c>
+      <c r="C338" t="s">
+        <v>15</v>
+      </c>
+      <c r="D338" t="s">
+        <v>17</v>
+      </c>
+      <c r="E338" t="s">
+        <v>127</v>
+      </c>
+      <c r="F338" t="s">
+        <v>150</v>
+      </c>
+      <c r="H338" t="s">
+        <v>466</v>
+      </c>
+      <c r="I338" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="339" spans="1:9">
+      <c r="A339" s="1">
+        <v>337</v>
+      </c>
+      <c r="B339" s="2">
+        <v>42805</v>
+      </c>
+      <c r="C339" t="s">
+        <v>9</v>
+      </c>
+      <c r="D339" t="s">
+        <v>17</v>
+      </c>
+      <c r="E339" t="s">
+        <v>128</v>
+      </c>
+      <c r="F339" t="s">
+        <v>207</v>
+      </c>
+      <c r="H339" t="s">
+        <v>467</v>
+      </c>
+      <c r="I339" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="340" spans="1:9">
+      <c r="A340" s="1">
+        <v>338</v>
+      </c>
+      <c r="B340" s="2">
+        <v>42805</v>
+      </c>
+      <c r="C340" t="s">
+        <v>9</v>
+      </c>
+      <c r="D340" t="s">
+        <v>17</v>
+      </c>
+      <c r="E340" t="s">
+        <v>44</v>
+      </c>
+      <c r="H340" t="s">
+        <v>468</v>
+      </c>
+      <c r="I340" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="341" spans="1:9">
+      <c r="A341" s="1">
+        <v>339</v>
+      </c>
+      <c r="B341" s="2">
+        <v>42806</v>
+      </c>
+      <c r="C341" t="s">
+        <v>9</v>
+      </c>
+      <c r="D341" t="s">
+        <v>17</v>
+      </c>
+      <c r="E341" t="s">
+        <v>22</v>
+      </c>
+      <c r="F341" t="s">
+        <v>150</v>
+      </c>
+      <c r="H341" t="s">
+        <v>469</v>
+      </c>
+      <c r="I341" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="342" spans="1:9">
+      <c r="A342" s="1">
+        <v>340</v>
+      </c>
+      <c r="B342" s="2">
+        <v>42809</v>
+      </c>
+      <c r="C342" t="s">
+        <v>9</v>
+      </c>
+      <c r="D342" t="s">
+        <v>17</v>
+      </c>
+      <c r="E342" t="s">
+        <v>55</v>
+      </c>
+      <c r="H342" t="s">
+        <v>470</v>
+      </c>
+      <c r="I342" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="343" spans="1:9">
+      <c r="A343" s="1">
+        <v>341</v>
+      </c>
+      <c r="B343" s="2">
+        <v>42811</v>
+      </c>
+      <c r="C343" t="s">
+        <v>9</v>
+      </c>
+      <c r="D343" t="s">
+        <v>17</v>
+      </c>
+      <c r="E343" t="s">
+        <v>22</v>
+      </c>
+      <c r="F343" t="s">
+        <v>150</v>
+      </c>
+      <c r="H343" t="s">
+        <v>471</v>
+      </c>
+      <c r="I343" t="s">
+        <v>473</v>
       </c>
     </row>
   </sheetData>

</xml_diff>